<commit_message>
defined Role, Team and their connections. added to data collector. added User and functions attributes
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Projects" sheetId="3" r:id="rId3"/>
+    <sheet name="Teams" sheetId="4" r:id="rId4"/>
+    <sheet name="Roles" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
   <si>
     <t>callback</t>
   </si>
@@ -223,13 +225,157 @@
   </si>
   <si>
     <t>user_name</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>WEB</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>BACKEND</t>
+  </si>
+  <si>
+    <t>project_name</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>users</t>
+  </si>
+  <si>
+    <t>team_name</t>
+  </si>
+  <si>
+    <t>ATEAM</t>
+  </si>
+  <si>
+    <t>ANAVNGERS</t>
+  </si>
+  <si>
+    <t>JusticLeage</t>
+  </si>
+  <si>
+    <t>OldTimers</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>max_priority</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>password_sha1</t>
+  </si>
+  <si>
+    <t>role_name</t>
+  </si>
+  <si>
+    <t>Magician</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Juggler</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>nami</t>
+  </si>
+  <si>
+    <t>goldi</t>
+  </si>
+  <si>
+    <t>locks</t>
+  </si>
+  <si>
+    <t>super</t>
+  </si>
+  <si>
+    <t>man</t>
+  </si>
+  <si>
+    <t>frank</t>
+  </si>
+  <si>
+    <t>sinatra</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>parker</t>
+  </si>
+  <si>
+    <t>don’t</t>
+  </si>
+  <si>
+    <t>know</t>
+  </si>
+  <si>
+    <t>sha1</t>
+  </si>
+  <si>
+    <t>sha2</t>
+  </si>
+  <si>
+    <t>sha3</t>
+  </si>
+  <si>
+    <t>sha4</t>
+  </si>
+  <si>
+    <t>sha5</t>
+  </si>
+  <si>
+    <t>sha6</t>
+  </si>
+  <si>
+    <t>sha7</t>
+  </si>
+  <si>
+    <t>sha8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +385,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -263,9 +421,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -571,7 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -1031,84 +1195,463 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>101</v>
+      </c>
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+      <c r="J4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" t="s">
+        <v>104</v>
+      </c>
+      <c r="J7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1116,14 +1659,121 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
clear and insert params table
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="Projects" sheetId="3" r:id="rId3"/>
-    <sheet name="Teams" sheetId="4" r:id="rId4"/>
-    <sheet name="Roles" sheetId="5" r:id="rId5"/>
+    <sheet name="function_parameters" sheetId="6" r:id="rId3"/>
+    <sheet name="Projects" sheetId="3" r:id="rId4"/>
+    <sheet name="Teams" sheetId="4" r:id="rId5"/>
+    <sheet name="Roles" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
   <si>
     <t>callback</t>
   </si>
@@ -369,12 +370,42 @@
   </si>
   <si>
     <t>sha8</t>
+  </si>
+  <si>
+    <t>function_id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Octopus_Params</t>
+  </si>
+  <si>
+    <t>Sys_Params</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>DataFrame</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -432,6 +463,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,6 +475,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -489,7 +526,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -524,7 +561,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -736,7 +773,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -808,7 +845,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -856,7 +893,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -904,7 +941,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -952,7 +989,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1000,7 +1037,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -1048,7 +1085,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -1096,7 +1133,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
@@ -1144,7 +1181,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -1197,7 +1234,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1541,6 +1578,126 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.75" customWidth="1"/>
+    <col min="4" max="4" width="15.875" customWidth="1"/>
+    <col min="5" max="5" width="22.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="4">
+        <v>66</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1659,7 +1816,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -1720,7 +1877,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>

</xml_diff>

<commit_message>
added tree DB models and relationships
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="Projects" sheetId="3" r:id="rId4"/>
     <sheet name="Teams" sheetId="4" r:id="rId5"/>
     <sheet name="Roles" sheetId="5" r:id="rId6"/>
+    <sheet name="TreeStructre" sheetId="7" r:id="rId7"/>
+    <sheet name="Trees" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
   <si>
     <t>callback</t>
   </si>
@@ -400,13 +402,130 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>tree_id</t>
+  </si>
+  <si>
+    <t>here</t>
+  </si>
+  <si>
+    <t>some</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>really</t>
+  </si>
+  <si>
+    <t>want</t>
+  </si>
+  <si>
+    <t>you</t>
+  </si>
+  <si>
+    <t>save</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>simple</t>
+  </si>
+  <si>
+    <t>another</t>
+  </si>
+  <si>
+    <t>oneandonly</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>big tree</t>
+  </si>
+  <si>
+    <t>small tree</t>
+  </si>
+  <si>
+    <t>small tree2</t>
+  </si>
+  <si>
+    <t>null_tree</t>
+  </si>
+  <si>
+    <t>node_name</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>nodes</t>
+  </si>
+  <si>
+    <t>node_data</t>
+  </si>
+  <si>
+    <t>once</t>
+  </si>
+  <si>
+    <t>upon a time</t>
+  </si>
+  <si>
+    <t>there was</t>
+  </si>
+  <si>
+    <t>a little</t>
+  </si>
+  <si>
+    <t>girl name</t>
+  </si>
+  <si>
+    <t>snowwhite</t>
+  </si>
+  <si>
+    <t>dgdfg</t>
+  </si>
+  <si>
+    <t>dfgfd</t>
+  </si>
+  <si>
+    <t>ddd</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>aasssad</t>
+  </si>
+  <si>
+    <t>asdsad</t>
+  </si>
+  <si>
+    <t>daeee</t>
+  </si>
+  <si>
+    <t>rrrrr</t>
+  </si>
+  <si>
+    <t>ttt</t>
+  </si>
+  <si>
+    <t>ffffffs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -526,7 +645,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,10 +677,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -593,7 +711,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -769,14 +886,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
@@ -793,7 +910,7 @@
     <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="15">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -843,7 +960,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -891,7 +1008,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -939,7 +1056,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -987,7 +1104,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1035,7 +1152,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1083,7 +1200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1131,7 +1248,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1179,7 +1296,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1231,14 +1348,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
@@ -1252,7 +1369,7 @@
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1284,7 +1401,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1316,7 +1433,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1348,7 +1465,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1380,7 +1497,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1412,7 +1529,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1444,7 +1561,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1476,7 +1593,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1508,7 +1625,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1540,34 +1657,34 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="15">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="15">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:3" ht="15">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:3" ht="15">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:3" ht="15">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:3" ht="15">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:3" ht="15">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:3" ht="15">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:3" ht="15">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:3" ht="15">
       <c r="C24" s="3"/>
     </row>
   </sheetData>
@@ -1577,14 +1694,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.75" customWidth="1"/>
@@ -1592,7 +1709,7 @@
     <col min="5" max="5" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>63</v>
       </c>
@@ -1609,7 +1726,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -1622,7 +1739,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -1635,7 +1752,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>2</v>
@@ -1650,7 +1767,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -1663,7 +1780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -1676,7 +1793,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
@@ -1697,19 +1814,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1723,7 +1840,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1734,7 +1851,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1745,7 +1862,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1756,7 +1873,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1767,7 +1884,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1778,7 +1895,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1789,7 +1906,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1800,7 +1917,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1817,19 +1934,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1840,7 +1957,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1848,7 +1965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1856,7 +1973,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1864,7 +1981,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1878,16 +1995,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1898,7 +2015,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1906,7 +2023,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1914,7 +2031,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1922,12 +2039,472 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>133</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>130</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E13" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>138</v>
+      </c>
+      <c r="E15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>164</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" t="s">
+        <v>165</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added groups model with relationship
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="Roles" sheetId="5" r:id="rId6"/>
     <sheet name="TreeStructre" sheetId="7" r:id="rId7"/>
     <sheet name="Trees" sheetId="8" r:id="rId8"/>
+    <sheet name="Groups" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
   <si>
     <t>callback</t>
   </si>
@@ -519,6 +520,18 @@
   </si>
   <si>
     <t>ffffffs</t>
+  </si>
+  <si>
+    <t>group1</t>
+  </si>
+  <si>
+    <t>group2</t>
+  </si>
+  <si>
+    <t>group3</t>
+  </si>
+  <si>
+    <t>group_name</t>
   </si>
 </sst>
 </file>
@@ -2056,7 +2069,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -2510,4 +2523,51 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
orm working for postgreSQL and MySQL
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="169">
   <si>
     <t>callback</t>
   </si>
@@ -207,12 +207,6 @@
     <t>is_locked</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -532,6 +526,9 @@
   </si>
   <si>
     <t>group_name</t>
+  </si>
+  <si>
+    <t>message</t>
   </si>
 </sst>
 </file>
@@ -902,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -925,10 +922,10 @@
   <sheetData>
     <row r="1" spans="1:16" ht="15">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -997,7 +994,7 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
         <v>33</v>
@@ -1017,8 +1014,8 @@
       <c r="O2" t="s">
         <v>46</v>
       </c>
-      <c r="P2" t="s">
-        <v>61</v>
+      <c r="P2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1045,7 +1042,7 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J3" t="s">
         <v>34</v>
@@ -1065,8 +1062,8 @@
       <c r="O3" t="s">
         <v>47</v>
       </c>
-      <c r="P3" t="s">
-        <v>62</v>
+      <c r="P3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1093,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J4" t="s">
         <v>35</v>
@@ -1113,8 +1110,8 @@
       <c r="O4" t="s">
         <v>48</v>
       </c>
-      <c r="P4" t="s">
-        <v>61</v>
+      <c r="P4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1141,7 +1138,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J5" t="s">
         <v>36</v>
@@ -1161,8 +1158,8 @@
       <c r="O5" t="s">
         <v>49</v>
       </c>
-      <c r="P5" t="s">
-        <v>62</v>
+      <c r="P5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1189,7 +1186,7 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J6" t="s">
         <v>37</v>
@@ -1209,8 +1206,8 @@
       <c r="O6" t="s">
         <v>40</v>
       </c>
-      <c r="P6" t="s">
-        <v>61</v>
+      <c r="P6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1237,7 +1234,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
@@ -1257,8 +1254,8 @@
       <c r="O7" t="s">
         <v>40</v>
       </c>
-      <c r="P7" t="s">
-        <v>62</v>
+      <c r="P7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1285,7 +1282,7 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J8" t="s">
         <v>38</v>
@@ -1305,8 +1302,8 @@
       <c r="O8" t="s">
         <v>41</v>
       </c>
-      <c r="P8" t="s">
-        <v>61</v>
+      <c r="P8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1333,7 +1330,7 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="J9" t="s">
         <v>39</v>
@@ -1344,14 +1341,17 @@
       <c r="L9">
         <v>7</v>
       </c>
+      <c r="M9" t="s">
+        <v>168</v>
+      </c>
       <c r="N9" t="s">
         <v>43</v>
       </c>
       <c r="O9" t="s">
         <v>41</v>
       </c>
-      <c r="P9" t="s">
-        <v>62</v>
+      <c r="P9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1384,34 +1384,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>89</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>90</v>
-      </c>
-      <c r="I1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1440,10 +1440,10 @@
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1469,13 +1469,13 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1501,13 +1501,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1533,13 +1533,13 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I5" t="s">
         <v>31</v>
       </c>
       <c r="J5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1568,10 +1568,10 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1597,13 +1597,13 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1629,13 +1629,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1661,13 +1661,13 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15">
@@ -1711,7 +1711,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1724,19 +1724,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1745,11 +1745,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D2" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
       <c r="E2" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1758,11 +1760,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2</v>
+      </c>
       <c r="E3" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1771,13 +1775,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1786,11 +1790,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D5" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1799,11 +1805,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="D6" s="4">
+        <v>4</v>
+      </c>
       <c r="E6" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1812,13 +1820,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D7" s="4">
         <v>66</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1841,16 +1849,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
         <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1858,10 +1866,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1869,10 +1877,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1880,10 +1888,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1891,10 +1899,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1902,10 +1910,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1913,10 +1921,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1924,10 +1932,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1935,10 +1943,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1961,13 +1969,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1975,7 +1983,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1983,7 +1991,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1991,7 +1999,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1999,7 +2007,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2019,13 +2027,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2033,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2041,7 +2049,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2049,7 +2057,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2057,7 +2065,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2077,22 +2085,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2106,10 +2114,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2129,7 +2137,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2146,10 +2154,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2166,10 +2174,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2189,7 +2197,7 @@
         <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2206,10 +2214,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -2226,10 +2234,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2246,10 +2254,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2266,10 +2274,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2286,10 +2294,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -2306,10 +2314,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2326,10 +2334,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2349,7 +2357,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2366,10 +2374,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2386,10 +2394,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2409,7 +2417,7 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2426,10 +2434,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2452,16 +2460,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2469,7 +2477,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2483,7 +2491,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2497,7 +2505,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2511,7 +2519,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2529,7 +2537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2537,10 +2545,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2548,7 +2556,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2556,7 +2564,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2564,7 +2572,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OctopusFunction run method in progress
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="177">
   <si>
     <t>callback</t>
   </si>
@@ -75,27 +75,6 @@
     <t>car</t>
   </si>
   <si>
-    <t>there.py</t>
-  </si>
-  <si>
-    <t>is.m</t>
-  </si>
-  <si>
-    <t>a.sql</t>
-  </si>
-  <si>
-    <t>lion.py</t>
-  </si>
-  <si>
-    <t>get.m</t>
-  </si>
-  <si>
-    <t>into.sql</t>
-  </si>
-  <si>
-    <t>the.py</t>
-  </si>
-  <si>
     <t>car.m</t>
   </si>
   <si>
@@ -529,6 +508,51 @@
   </si>
   <si>
     <t>message</t>
+  </si>
+  <si>
+    <t>C:\Git_Rep\Development\Functions</t>
+  </si>
+  <si>
+    <t>some_functions.py</t>
+  </si>
+  <si>
+    <t>calc.py</t>
+  </si>
+  <si>
+    <t>file_name</t>
+  </si>
+  <si>
+    <t>plus_func</t>
+  </si>
+  <si>
+    <t>multi_func</t>
+  </si>
+  <si>
+    <t>return_success</t>
+  </si>
+  <si>
+    <t>return_warning</t>
+  </si>
+  <si>
+    <t>return_fail</t>
+  </si>
+  <si>
+    <t>return_error</t>
+  </si>
+  <si>
+    <t>return_nodata</t>
+  </si>
+  <si>
+    <t>bla.py</t>
+  </si>
+  <si>
+    <t>is_class_method</t>
+  </si>
+  <si>
+    <t>class_name</t>
+  </si>
+  <si>
+    <t>Calc</t>
   </si>
 </sst>
 </file>
@@ -581,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -595,6 +619,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -897,80 +923,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.375" customWidth="1"/>
-    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.375" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:19" ht="15">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O1" t="s">
         <v>51</v>
       </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
-        <v>59</v>
-      </c>
       <c r="P1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+        <v>52</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="S1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -978,47 +1014,55 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="str">
-        <f>CONCATENATE("c:/functions/",C2)</f>
-        <v>c:/functions/there.py</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+        <v>166</v>
+      </c>
+      <c r="D2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E2" t="s">
+        <v>162</v>
       </c>
       <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J2" t="s">
-        <v>33</v>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2" t="s">
-        <v>52</v>
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
       </c>
       <c r="N2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O2" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2">
+      <c r="P2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1026,95 +1070,109 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D9" si="0">CONCATENATE("c:/functions/",C3)</f>
-        <v>c:/functions/is.m</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>167</v>
+      </c>
+      <c r="D3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E3" t="s">
+        <v>162</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>57</v>
       </c>
       <c r="K3" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
       </c>
       <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
         <v>40</v>
       </c>
-      <c r="O3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>c:/functions/a.sql</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="C4" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="D4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>35</v>
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
-        <v>54</v>
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4">
+        <v>2</v>
       </c>
       <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
         <v>41</v>
       </c>
-      <c r="O4" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4">
+      <c r="Q4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1122,47 +1180,52 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>c:/functions/lion.py</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E5" t="s">
+        <v>162</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" t="s">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" t="s">
+        <v>56</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
-      </c>
-      <c r="L5">
-        <v>3</v>
-      </c>
-      <c r="M5" t="s">
-        <v>55</v>
+        <v>29</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
       </c>
       <c r="N5" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" t="s">
         <v>42</v>
       </c>
-      <c r="O5" t="s">
-        <v>49</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1170,47 +1233,52 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>c:/functions/get.m</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" t="s">
+        <v>162</v>
       </c>
       <c r="F6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" t="s">
         <v>37</v>
       </c>
-      <c r="K6" t="s">
-        <v>44</v>
-      </c>
-      <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
-        <v>57</v>
+      <c r="M6">
+        <v>4</v>
       </c>
       <c r="N6" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="O6" t="s">
-        <v>40</v>
-      </c>
-      <c r="P6">
+        <v>35</v>
+      </c>
+      <c r="P6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1218,47 +1286,52 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>c:/functions/into.sql</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
+        <v>171</v>
+      </c>
+      <c r="D7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" t="s">
+        <v>162</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
         <v>6</v>
       </c>
-      <c r="H7" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" t="s">
         <v>7</v>
       </c>
-      <c r="K7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7">
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7">
         <v>5</v>
-      </c>
-      <c r="M7" t="s">
-        <v>13</v>
       </c>
       <c r="N7" t="s">
         <v>13</v>
       </c>
       <c r="O7" t="s">
-        <v>40</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
+        <v>13</v>
+      </c>
+      <c r="P7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1266,47 +1339,53 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>c:/functions/the.py</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
+        <v>172</v>
+      </c>
+      <c r="D8" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" t="str">
+        <f>CONCATENATE("c:/functions/",C8)</f>
+        <v>c:/functions/return_nodata</v>
       </c>
       <c r="F8">
         <v>6</v>
       </c>
       <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
         <v>7</v>
       </c>
-      <c r="H8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" t="s">
+      <c r="I8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" t="s">
         <v>38</v>
       </c>
-      <c r="K8" t="s">
-        <v>45</v>
-      </c>
-      <c r="L8">
+      <c r="M8">
         <v>6</v>
       </c>
-      <c r="M8" t="s">
-        <v>56</v>
-      </c>
       <c r="N8" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="O8" t="s">
-        <v>41</v>
-      </c>
-      <c r="P8">
+        <v>35</v>
+      </c>
+      <c r="P8" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1314,44 +1393,50 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" t="str">
+        <f>CONCATENATE("c:/functions/",C9)</f>
         <v>c:/functions/car.m</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
       <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="G9">
         <v>7</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>8</v>
       </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-      <c r="J9" t="s">
-        <v>39</v>
+      <c r="I9" t="s">
+        <v>57</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9">
+        <v>32</v>
+      </c>
+      <c r="L9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9">
         <v>7</v>
       </c>
-      <c r="M9" t="s">
-        <v>168</v>
-      </c>
       <c r="N9" t="s">
-        <v>43</v>
+        <v>161</v>
       </c>
       <c r="O9" t="s">
-        <v>41</v>
-      </c>
-      <c r="P9">
-        <v>1</v>
+        <v>36</v>
+      </c>
+      <c r="P9" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1384,34 +1469,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
         <v>81</v>
       </c>
-      <c r="E1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H1" t="s">
-        <v>88</v>
-      </c>
       <c r="I1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1419,7 +1504,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1437,13 +1522,13 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1451,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1469,13 +1554,13 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1483,7 +1568,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -1501,13 +1586,13 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1515,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -1533,13 +1618,13 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -1547,7 +1632,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1565,13 +1650,13 @@
         <v>5</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1579,7 +1664,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -1597,13 +1682,13 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="I7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="J7" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1611,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -1629,13 +1714,13 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I8" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="J8" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1643,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1661,13 +1746,13 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="I9" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15">
@@ -1724,19 +1809,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1745,13 +1830,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1760,13 +1845,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1775,13 +1860,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1790,13 +1875,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1805,13 +1890,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D6" s="4">
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1820,13 +1905,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D7" s="4">
         <v>66</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -1849,16 +1934,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1866,10 +1951,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1877,10 +1962,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1888,10 +1973,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1899,10 +1984,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1910,10 +1995,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1921,10 +2006,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1932,10 +2017,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1943,10 +2028,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1969,13 +2054,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1983,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1991,7 +2076,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1999,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2007,7 +2092,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2027,13 +2112,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2041,7 +2126,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2049,7 +2134,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2057,7 +2142,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2065,7 +2150,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2085,22 +2170,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="F1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2114,10 +2199,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2137,7 +2222,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2154,10 +2239,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E4" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2174,10 +2259,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2194,10 +2279,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2214,10 +2299,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E7" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -2234,10 +2319,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E8" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2254,10 +2339,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E9" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2274,10 +2359,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="E10" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2294,10 +2379,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E11" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -2314,10 +2399,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2334,10 +2419,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2357,7 +2442,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2374,10 +2459,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2394,10 +2479,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E16" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2417,7 +2502,7 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2434,10 +2519,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2460,16 +2545,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1" t="s">
         <v>139</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2477,7 +2562,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2491,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2505,7 +2590,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2519,7 +2604,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2545,10 +2630,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2556,7 +2641,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2564,7 +2649,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2572,7 +2657,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functions run model working
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Functions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="177">
   <si>
     <t>callback</t>
   </si>
@@ -366,15 +366,9 @@
     <t>text</t>
   </si>
   <si>
-    <t>ENG</t>
-  </si>
-  <si>
     <t>DataFrame</t>
   </si>
   <si>
-    <t>String</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -553,6 +547,12 @@
   </si>
   <si>
     <t>Calc</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
@@ -925,8 +925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1000,10 +1000,10 @@
         <v>53</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="S1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1014,13 +1014,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1070,13 +1070,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1115,7 +1115,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15">
@@ -1126,13 +1126,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1180,13 +1180,13 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1233,13 +1233,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1286,13 +1286,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1339,10 +1339,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E8" t="str">
         <f>CONCATENATE("c:/functions/",C8)</f>
@@ -1396,7 +1396,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E9" t="str">
         <f>CONCATENATE("c:/functions/",C9)</f>
@@ -1424,7 +1424,7 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="O9" t="s">
         <v>36</v>
@@ -1793,10 +1793,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1830,13 +1830,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1845,13 +1845,13 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D3" s="4">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>115</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1860,13 +1860,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1881,7 +1881,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1896,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1911,7 +1911,21 @@
         <v>66</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -2173,19 +2187,19 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2199,10 +2213,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2222,7 +2236,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2239,10 +2253,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2259,10 +2273,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2282,7 +2296,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2299,10 +2313,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -2319,10 +2333,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2339,10 +2353,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2359,10 +2373,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2379,10 +2393,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -2399,10 +2413,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2419,10 +2433,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2442,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2459,10 +2473,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2479,10 +2493,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2502,7 +2516,7 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2519,10 +2533,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2548,13 +2562,13 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2562,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2576,7 +2590,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2590,7 +2604,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2604,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2633,7 +2647,7 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2641,7 +2655,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2649,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2657,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
api supports results by mission id and result id
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="178">
   <si>
     <t>callback</t>
   </si>
@@ -357,9 +357,6 @@
     <t>value</t>
   </si>
   <si>
-    <t>Octopus_Params</t>
-  </si>
-  <si>
     <t>Sys_Params</t>
   </si>
   <si>
@@ -552,7 +549,13 @@
     <t>int</t>
   </si>
   <si>
-    <t>float</t>
+    <t>Tests_Params</t>
+  </si>
+  <si>
+    <t>__</t>
+  </si>
+  <si>
+    <t>param_index</t>
   </si>
 </sst>
 </file>
@@ -958,7 +961,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -1000,10 +1003,10 @@
         <v>53</v>
       </c>
       <c r="R1" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="S1" t="s">
         <v>172</v>
-      </c>
-      <c r="S1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1014,13 +1017,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1059,7 +1062,7 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -1070,13 +1073,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -1115,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15">
@@ -1126,13 +1129,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -1180,13 +1183,13 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1233,13 +1236,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1286,13 +1289,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1339,10 +1342,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E8" t="str">
         <f>CONCATENATE("c:/functions/",C8)</f>
@@ -1396,7 +1399,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E9" t="str">
         <f>CONCATENATE("c:/functions/",C9)</f>
@@ -1424,7 +1427,7 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O9" t="s">
         <v>36</v>
@@ -1793,21 +1796,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="15.875" customWidth="1"/>
-    <col min="5" max="5" width="22.25" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -1815,117 +1819,175 @@
         <v>108</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D3" s="4">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D4" s="4">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3</v>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>175</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>176</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D6" s="4">
-        <v>4</v>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>176</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="4">
         <v>66</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" s="4">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="4">
-        <v>5.5</v>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>176</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2187,19 +2249,19 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2213,10 +2275,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -2236,7 +2298,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2253,10 +2315,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2273,10 +2335,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -2296,7 +2358,7 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -2313,10 +2375,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F7">
         <v>4</v>
@@ -2333,10 +2395,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F8">
         <v>4</v>
@@ -2353,10 +2415,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -2373,10 +2435,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -2393,10 +2455,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F11">
         <v>7</v>
@@ -2413,10 +2475,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -2433,10 +2495,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2456,7 +2518,7 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2473,10 +2535,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E15" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -2493,10 +2555,10 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2516,7 +2578,7 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17">
         <v>2</v>
@@ -2533,10 +2595,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2562,13 +2624,13 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
         <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2576,7 +2638,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2590,7 +2652,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2604,7 +2666,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2618,7 +2680,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2647,7 +2709,7 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2655,7 +2717,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2663,7 +2725,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2671,7 +2733,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished htmls and definition of tables in excel
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,25 +4,34 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="929" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="Functions" sheetId="1" r:id="rId1"/>
-    <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="function_parameters" sheetId="6" r:id="rId3"/>
-    <sheet name="Projects" sheetId="3" r:id="rId4"/>
-    <sheet name="Teams" sheetId="4" r:id="rId5"/>
-    <sheet name="Roles" sheetId="5" r:id="rId6"/>
-    <sheet name="TreeStructre" sheetId="7" r:id="rId7"/>
-    <sheet name="Trees" sheetId="8" r:id="rId8"/>
-    <sheet name="Groups" sheetId="9" r:id="rId9"/>
+    <sheet name="Projects" sheetId="3" r:id="rId1"/>
+    <sheet name="Sites" sheetId="10" r:id="rId2"/>
+    <sheet name="Complex_Net" sheetId="11" r:id="rId3"/>
+    <sheet name="NetConfig" sheetId="12" r:id="rId4"/>
+    <sheet name="NetSystems" sheetId="13" r:id="rId5"/>
+    <sheet name="Process" sheetId="17" r:id="rId6"/>
+    <sheet name="Stage" sheetId="14" r:id="rId7"/>
+    <sheet name="Stage_RunSystem" sheetId="15" r:id="rId8"/>
+    <sheet name="Stage_Analyse" sheetId="16" r:id="rId9"/>
+    <sheet name="Run_System_Tasks" sheetId="18" r:id="rId10"/>
+    <sheet name="Users" sheetId="2" r:id="rId11"/>
+    <sheet name="function_parameters" sheetId="6" r:id="rId12"/>
+    <sheet name="Functions" sheetId="1" r:id="rId13"/>
+    <sheet name="Teams" sheetId="4" r:id="rId14"/>
+    <sheet name="Roles" sheetId="5" r:id="rId15"/>
+    <sheet name="TreeStructre" sheetId="7" r:id="rId16"/>
+    <sheet name="Trees" sheetId="8" r:id="rId17"/>
+    <sheet name="Groups" sheetId="9" r:id="rId18"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="239">
   <si>
     <t>callback</t>
   </si>
@@ -556,6 +565,189 @@
   </si>
   <si>
     <t>param_index</t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>output_dir</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>site_ip</t>
+  </si>
+  <si>
+    <t>auto_data_db_ip</t>
+  </si>
+  <si>
+    <t>auto_data_site_ip</t>
+  </si>
+  <si>
+    <t>execrsice_db_ip</t>
+  </si>
+  <si>
+    <t>execrsice_site_ip</t>
+  </si>
+  <si>
+    <t>site_db_ip</t>
+  </si>
+  <si>
+    <t>nets</t>
+  </si>
+  <si>
+    <t>stations</t>
+  </si>
+  <si>
+    <t>project_id</t>
+  </si>
+  <si>
+    <t>changed_date</t>
+  </si>
+  <si>
+    <t>changed_by</t>
+  </si>
+  <si>
+    <t>Kind</t>
+  </si>
+  <si>
+    <t>config_id</t>
+  </si>
+  <si>
+    <t>Systems_id</t>
+  </si>
+  <si>
+    <t>ilan</t>
+  </si>
+  <si>
+    <t>Project_id</t>
+  </si>
+  <si>
+    <t>Lnk_System</t>
+  </si>
+  <si>
+    <t>Link_Ext_Simulation</t>
+  </si>
+  <si>
+    <t>Complex_Net_ID</t>
+  </si>
+  <si>
+    <t>Smiulation_Watch</t>
+  </si>
+  <si>
+    <t>Simulation_Dis</t>
+  </si>
+  <si>
+    <t>Simulation_Ext_Flag</t>
+  </si>
+  <si>
+    <t>Backup_Env</t>
+  </si>
+  <si>
+    <t>Backup_Env_Ext_Flag</t>
+  </si>
+  <si>
+    <t>System_Type</t>
+  </si>
+  <si>
+    <t>System_Num</t>
+  </si>
+  <si>
+    <t>process_id</t>
+  </si>
+  <si>
+    <t>processes_id</t>
+  </si>
+  <si>
+    <t>names</t>
+  </si>
+  <si>
+    <t>concequences</t>
+  </si>
+  <si>
+    <t>change_date</t>
+  </si>
+  <si>
+    <t>net</t>
+  </si>
+  <si>
+    <t>complex_net_id</t>
+  </si>
+  <si>
+    <t>Site_id</t>
+  </si>
+  <si>
+    <t>scenario_folder</t>
+  </si>
+  <si>
+    <t>scenario_file</t>
+  </si>
+  <si>
+    <t>Is_Run_All_Scenarios</t>
+  </si>
+  <si>
+    <t>DP_Folder</t>
+  </si>
+  <si>
+    <t>DP_File</t>
+  </si>
+  <si>
+    <t>OVR_File</t>
+  </si>
+  <si>
+    <t>RunTime</t>
+  </si>
+  <si>
+    <t>IsAutoUserCmd</t>
+  </si>
+  <si>
+    <t>AutoUserCmd_File</t>
+  </si>
+  <si>
+    <t>IsFMC</t>
+  </si>
+  <si>
+    <t>FMC_Connection_File</t>
+  </si>
+  <si>
+    <t>FMC_Scenario_File</t>
+  </si>
+  <si>
+    <t>FMC_Config_File</t>
+  </si>
+  <si>
+    <t>IsEvn_Shut_Down</t>
+  </si>
+  <si>
+    <t>Evn_Shut_Down_Time</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>List_Analyze_Name</t>
+  </si>
+  <si>
+    <t>Analyze_Type</t>
+  </si>
+  <si>
+    <t>stage_id</t>
+  </si>
+  <si>
+    <t>stage_type</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>mission_id</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>IsFit</t>
   </si>
 </sst>
 </file>
@@ -588,12 +780,30 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -608,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -624,6 +834,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,6 +1148,764 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G24" sqref="B24:G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2">
+        <v>200</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>96</v>
+      </c>
+      <c r="I8" t="s">
+        <v>97</v>
+      </c>
+      <c r="J8" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15">
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="15">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="3:3" ht="15">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:3" ht="15">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3" ht="15">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3" ht="15">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3" ht="15">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3" ht="15">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3" ht="15">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3" ht="15">
+      <c r="C24" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E7" s="4">
+        <v>66</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="4">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="B9" s="4">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="B10" s="4">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1448,674 +2428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>89</v>
-      </c>
-      <c r="J2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="s">
-        <v>92</v>
-      </c>
-      <c r="I4" t="s">
-        <v>93</v>
-      </c>
-      <c r="J4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" t="s">
-        <v>95</v>
-      </c>
-      <c r="J7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8">
-        <v>7</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>7</v>
-      </c>
-      <c r="H8" t="s">
-        <v>96</v>
-      </c>
-      <c r="I8" t="s">
-        <v>97</v>
-      </c>
-      <c r="J8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>98</v>
-      </c>
-      <c r="I9" t="s">
-        <v>99</v>
-      </c>
-      <c r="J9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="15">
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="3:3" ht="15">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="3:3" ht="15">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="3:3" ht="15">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="3:3" ht="15">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="3:3" ht="15">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="3:3" ht="15">
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="3:3" ht="15">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="3:3" ht="15">
-      <c r="C24" s="3"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="22.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" s="4">
-        <v>2</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" s="4">
-        <v>4</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4">
-        <v>5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E7" s="4">
-        <v>66</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="B8" s="4">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4">
-        <v>2</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4">
-        <v>2</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" s="4">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2176,7 +2489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2234,7 +2547,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -2609,7 +2922,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2694,7 +3007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2739,4 +3052,480 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" t="s">
+        <v>186</v>
+      </c>
+      <c r="H1" t="s">
+        <v>185</v>
+      </c>
+      <c r="I1" t="s">
+        <v>184</v>
+      </c>
+      <c r="J1" t="s">
+        <v>183</v>
+      </c>
+      <c r="K1" t="s">
+        <v>182</v>
+      </c>
+      <c r="L1" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" t="s">
+        <v>188</v>
+      </c>
+      <c r="N1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="11" customFormat="1">
+      <c r="A1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" t="s">
+        <v>204</v>
+      </c>
+      <c r="I1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="7" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="9" customFormat="1">
+      <c r="A1" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:S1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="6" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel for new tables and api functions
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -4,34 +4,37 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="929" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="929" firstSheet="8" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projects" sheetId="3" r:id="rId1"/>
-    <sheet name="Sites" sheetId="10" r:id="rId2"/>
-    <sheet name="Complex_Net" sheetId="11" r:id="rId3"/>
-    <sheet name="NetConfig" sheetId="12" r:id="rId4"/>
-    <sheet name="NetSystems" sheetId="13" r:id="rId5"/>
-    <sheet name="Process" sheetId="17" r:id="rId6"/>
-    <sheet name="Stage" sheetId="14" r:id="rId7"/>
-    <sheet name="Stage_RunSystem" sheetId="15" r:id="rId8"/>
-    <sheet name="Stage_Analyse" sheetId="16" r:id="rId9"/>
-    <sheet name="Run_System_Tasks" sheetId="18" r:id="rId10"/>
-    <sheet name="Users" sheetId="2" r:id="rId11"/>
-    <sheet name="function_parameters" sheetId="6" r:id="rId12"/>
-    <sheet name="Functions" sheetId="1" r:id="rId13"/>
-    <sheet name="Teams" sheetId="4" r:id="rId14"/>
-    <sheet name="Roles" sheetId="5" r:id="rId15"/>
-    <sheet name="TreeStructre" sheetId="7" r:id="rId16"/>
-    <sheet name="Trees" sheetId="8" r:id="rId17"/>
-    <sheet name="Groups" sheetId="9" r:id="rId18"/>
+    <sheet name="Sheet3" sheetId="21" r:id="rId2"/>
+    <sheet name="Sites" sheetId="10" r:id="rId3"/>
+    <sheet name="Complex_Net" sheetId="11" r:id="rId4"/>
+    <sheet name="NetConfig" sheetId="12" r:id="rId5"/>
+    <sheet name="NetSystems" sheetId="13" r:id="rId6"/>
+    <sheet name="Process" sheetId="17" r:id="rId7"/>
+    <sheet name="Stage" sheetId="14" r:id="rId8"/>
+    <sheet name="Stage_Run_Mani" sheetId="15" r:id="rId9"/>
+    <sheet name="Stage_Analyse" sheetId="16" r:id="rId10"/>
+    <sheet name="Mission" sheetId="18" r:id="rId11"/>
+    <sheet name="Run_System_Task" sheetId="19" r:id="rId12"/>
+    <sheet name="Analyse_Task" sheetId="20" r:id="rId13"/>
+    <sheet name="Users" sheetId="2" r:id="rId14"/>
+    <sheet name="function_parameters" sheetId="6" r:id="rId15"/>
+    <sheet name="Functions" sheetId="1" r:id="rId16"/>
+    <sheet name="Teams" sheetId="4" r:id="rId17"/>
+    <sheet name="Roles" sheetId="5" r:id="rId18"/>
+    <sheet name="TreeStructre" sheetId="7" r:id="rId19"/>
+    <sheet name="Trees" sheetId="8" r:id="rId20"/>
+    <sheet name="Groups" sheetId="9" r:id="rId21"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="305">
   <si>
     <t>callback</t>
   </si>
@@ -618,9 +621,6 @@
     <t>Systems_id</t>
   </si>
   <si>
-    <t>ilan</t>
-  </si>
-  <si>
     <t>Project_id</t>
   </si>
   <si>
@@ -654,9 +654,6 @@
     <t>System_Num</t>
   </si>
   <si>
-    <t>process_id</t>
-  </si>
-  <si>
     <t>processes_id</t>
   </si>
   <si>
@@ -748,13 +745,339 @@
   </si>
   <si>
     <t>IsFit</t>
+  </si>
+  <si>
+    <t>ID שמציין מה התהליך כולו</t>
+  </si>
+  <si>
+    <t>ID  עבור הרצת מני</t>
+  </si>
+  <si>
+    <t>ID הניתוח</t>
+  </si>
+  <si>
+    <t xml:space="preserve">תעשה ניתוח של קבוצה </t>
+  </si>
+  <si>
+    <t>תעשה פונ 1</t>
+  </si>
+  <si>
+    <t>תעשה פונ 2</t>
+  </si>
+  <si>
+    <t>process_id הגדרה</t>
+  </si>
+  <si>
+    <t>mission_ID ביצוע</t>
+  </si>
+  <si>
+    <t>RunSystemTaskID</t>
+  </si>
+  <si>
+    <t>AnalzeTaskID</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>עבור המקרה הרגיל:</t>
+  </si>
+  <si>
+    <t>עבור המקרה כיול פרמטרים:</t>
+  </si>
+  <si>
+    <t>FitKind</t>
+  </si>
+  <si>
+    <t>Run_System_ID</t>
+  </si>
+  <si>
+    <t>Stage_ID</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>מבטא את סוג השלב</t>
+  </si>
+  <si>
+    <t>במקרה של הרצת מערכת</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סוג השלב יפנה למערכת הרלוונטית לדומא: </t>
+  </si>
+  <si>
+    <t>Run_Mani_System</t>
+  </si>
+  <si>
+    <t>content_id</t>
+  </si>
+  <si>
+    <t>מקשר לטבלאות של "הבנים":
+ Stage_Run_Mani" Stage_Run_Shaked</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Run_ID</t>
+  </si>
+  <si>
+    <t>Start_Run_Time</t>
+  </si>
+  <si>
+    <t>End_Run_Time</t>
+  </si>
+  <si>
+    <t>Rejected Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start_Time </t>
+  </si>
+  <si>
+    <t>End Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ddmmyy hh mm ss </t>
+  </si>
+  <si>
+    <t>מקרה "מורכב" / הרצה של 2 מערכות שונות במקביל, כאשר הניתוח הן רלוונטים לכול מערכת בנפרד</t>
+  </si>
+  <si>
+    <t>777-710</t>
+  </si>
+  <si>
+    <t>run_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>השדה יכול להיות Null</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ניתוח כתוצאה מהרצת תהליך </t>
+  </si>
+  <si>
+    <t>ניתוח כתוצאה מהרצת פונקציות שמקושרות לריצות (מסך ה RunAnalyze)</t>
+  </si>
+  <si>
+    <t>מטרת הטבלה לנהל תהליכי ניתוח שמגיעים משני מקורות שונים:</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status_Analyse</t>
+  </si>
+  <si>
+    <t>Result_ID</t>
+  </si>
+  <si>
+    <t>#status</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#0 - created</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#1 - failure pushing to tasks queue</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#2 - in tasks_queue</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#3 - faiiure running task</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#4 - task done. waiting to be written to db</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#5 - failure writing to db</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#6 - results in db</t>
+    </r>
+  </si>
+  <si>
+    <t>מטרת הטבלה לנהל בקשות להרצה / ניתוח שמגיעים משני מקורות שונים:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מסך Define_Processהרצת תהליך </t>
+  </si>
+  <si>
+    <t>מסך ה RunAnalyze</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#2 - in process</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#3 - </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#1 - Error</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF6A9955"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>#4 - done</t>
+    </r>
+  </si>
+  <si>
+    <t>Analyse_Task_ID</t>
+  </si>
+  <si>
+    <t>api/class_name/function/paramters</t>
+  </si>
+  <si>
+    <t>save(data)</t>
+  </si>
+  <si>
+    <t>delete(id)</t>
+  </si>
+  <si>
+    <t>update(id,data)</t>
+  </si>
+  <si>
+    <t>get_by_ids(ids,filter)</t>
+  </si>
+  <si>
+    <t>get_by_names(names,filter)</t>
+  </si>
+  <si>
+    <t>get_names(filter)</t>
+  </si>
+  <si>
+    <t>get_ids(filter)</t>
+  </si>
+  <si>
+    <t>filter - json project:, owner:,tags:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,8 +1102,28 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF6A9955"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,8 +1148,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -814,11 +1205,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -844,6 +1315,65 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1294,17 +1824,16 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFFF0000"/>
+    <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
@@ -1312,44 +1841,16 @@
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>236</v>
+        <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>123</v>
-      </c>
-      <c r="B2" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>123</v>
-      </c>
-      <c r="B3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3">
-        <v>200</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1358,6 +1859,1395 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:L68"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A1" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18.75">
+      <c r="A2" s="13">
+        <v>123</v>
+      </c>
+      <c r="B2">
+        <v>4444</v>
+      </c>
+      <c r="E2">
+        <v>200</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="53" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A3">
+        <v>333</v>
+      </c>
+      <c r="B3">
+        <v>4445</v>
+      </c>
+      <c r="E3">
+        <v>333</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" s="54" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18.75">
+      <c r="A4" s="26">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>4446</v>
+      </c>
+      <c r="E4">
+        <v>400</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75">
+      <c r="H5" s="54" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18.75">
+      <c r="H6" s="54" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18.75">
+      <c r="H7" s="54" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
+      <c r="F8" s="54"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75">
+      <c r="C9" s="31" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="F9" s="54"/>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1">
+      <c r="C10" s="42" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="C11" s="55"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:12" ht="15" thickBot="1">
+      <c r="C12" s="55"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="C14" s="47"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48" t="s">
+        <v>288</v>
+      </c>
+      <c r="H14" s="49"/>
+      <c r="J14" s="13" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48" t="s">
+        <v>289</v>
+      </c>
+      <c r="G15" s="48">
+        <v>1</v>
+      </c>
+      <c r="H15" s="49"/>
+      <c r="K15" s="15" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="C16" s="47"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="G16" s="48">
+        <v>2</v>
+      </c>
+      <c r="H16" s="49"/>
+      <c r="L16" s="16" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
+      <c r="L17" s="16"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+    </row>
+    <row r="21" spans="3:12" ht="15" thickBot="1">
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="52"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="55"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="55"/>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="C24" s="55"/>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="3:12" ht="15">
+      <c r="I25" s="30" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" ht="15" thickBot="1"/>
+    <row r="27" spans="3:12">
+      <c r="C27" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="26">
+        <v>123</v>
+      </c>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="18"/>
+    </row>
+    <row r="28" spans="3:12">
+      <c r="C28" s="19"/>
+      <c r="D28" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="27">
+        <v>666</v>
+      </c>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21"/>
+    </row>
+    <row r="29" spans="3:12">
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F29" s="28">
+        <v>777</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28">
+        <v>778</v>
+      </c>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28">
+        <v>779</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28">
+        <v>710</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="15" thickBot="1">
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="24"/>
+    </row>
+    <row r="35" spans="3:9" ht="15">
+      <c r="I35" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" ht="15" thickBot="1"/>
+    <row r="37" spans="3:9">
+      <c r="C37" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D37" s="26">
+        <v>333</v>
+      </c>
+      <c r="E37" s="17"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+    </row>
+    <row r="38" spans="3:9">
+      <c r="C38" s="19"/>
+      <c r="D38" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E38" s="27">
+        <v>680</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="21"/>
+    </row>
+    <row r="39" spans="3:9">
+      <c r="C39" s="19"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F39" s="28">
+        <v>800</v>
+      </c>
+      <c r="G39" s="20"/>
+      <c r="H39" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9">
+      <c r="C40" s="19"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28">
+        <v>801</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9">
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28">
+        <v>802</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H41" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9">
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28">
+        <v>803</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H42" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9">
+      <c r="C43" s="19"/>
+      <c r="D43" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E43" s="27">
+        <v>681</v>
+      </c>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
+    </row>
+    <row r="44" spans="3:9">
+      <c r="C44" s="19"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F44" s="28">
+        <v>803</v>
+      </c>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9">
+      <c r="C45" s="19"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="28">
+        <v>804</v>
+      </c>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9">
+      <c r="C46" s="19"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28">
+        <v>805</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H46" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" ht="15" thickBot="1">
+      <c r="C47" s="22"/>
+      <c r="D47" s="23"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="28">
+        <v>806</v>
+      </c>
+      <c r="G47" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="15" thickBot="1">
+      <c r="I51" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9">
+      <c r="C52" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D52" s="26">
+        <v>444</v>
+      </c>
+      <c r="E52" s="17"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="18"/>
+    </row>
+    <row r="53" spans="3:9">
+      <c r="C53" s="19"/>
+      <c r="D53" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E53" s="27">
+        <v>900</v>
+      </c>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="21"/>
+    </row>
+    <row r="54" spans="3:9">
+      <c r="C54" s="19"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F54" s="28">
+        <v>1001</v>
+      </c>
+      <c r="G54" s="20"/>
+      <c r="H54" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9">
+      <c r="C55" s="19"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28">
+        <v>1002</v>
+      </c>
+      <c r="G55" s="20"/>
+      <c r="H55" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9">
+      <c r="C56" s="19"/>
+      <c r="D56" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E56" s="27">
+        <v>901</v>
+      </c>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="21"/>
+    </row>
+    <row r="57" spans="3:9">
+      <c r="C57" s="19"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F57" s="28">
+        <v>1003</v>
+      </c>
+      <c r="G57" s="20"/>
+      <c r="H57" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" ht="15" thickBot="1">
+      <c r="C58" s="22"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29">
+        <v>1004</v>
+      </c>
+      <c r="G58" s="23"/>
+      <c r="H58" s="24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" ht="15" thickBot="1"/>
+    <row r="64" spans="3:9">
+      <c r="C64" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D64" s="26">
+        <v>200</v>
+      </c>
+      <c r="E64" s="17"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="18"/>
+    </row>
+    <row r="65" spans="3:8">
+      <c r="C65" s="19"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F65" s="28">
+        <v>2000</v>
+      </c>
+      <c r="G65" s="20"/>
+      <c r="H65" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8">
+      <c r="C66" s="19"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="28"/>
+      <c r="F66" s="28">
+        <v>2001</v>
+      </c>
+      <c r="G66" s="20"/>
+      <c r="H66" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8">
+      <c r="C67" s="19"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="28"/>
+      <c r="F67" s="28">
+        <v>2002</v>
+      </c>
+      <c r="G67" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H67" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" ht="15" thickBot="1">
+      <c r="C68" s="22"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="28">
+        <v>2003</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="9" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1" s="40" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="27">
+        <v>666</v>
+      </c>
+      <c r="B2" s="13">
+        <v>123</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="41" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
+      <c r="I9" s="30" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1"/>
+    <row r="11" spans="1:9">
+      <c r="C11" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D11" s="26">
+        <v>123</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="C12" s="19"/>
+      <c r="D12" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E12" s="27">
+        <v>666</v>
+      </c>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="C13" s="19"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F13" s="28">
+        <v>777</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="C14" s="19"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28">
+        <v>778</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="C15" s="19"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28">
+        <v>779</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="19"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28">
+        <v>710</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="15" thickBot="1">
+      <c r="C17" s="22"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="19" spans="3:9" ht="15">
+      <c r="I19" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="15" thickBot="1"/>
+    <row r="21" spans="3:9">
+      <c r="C21" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D21" s="26">
+        <v>333</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="3:9">
+      <c r="C22" s="19"/>
+      <c r="D22" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E22" s="27">
+        <v>680</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+    </row>
+    <row r="23" spans="3:9">
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F23" s="28">
+        <v>800</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9">
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28">
+        <v>801</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9">
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28">
+        <v>802</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9">
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28">
+        <v>803</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9">
+      <c r="C27" s="19"/>
+      <c r="D27" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E27" s="27">
+        <v>681</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="3:9">
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F28" s="28">
+        <v>803</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9">
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28">
+        <v>804</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9">
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28">
+        <v>805</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" ht="15" thickBot="1">
+      <c r="C31" s="22"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="28">
+        <v>806</v>
+      </c>
+      <c r="G31" s="23" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:L42"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="C1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D1" t="s">
+        <v>270</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F1" t="s">
+        <v>279</v>
+      </c>
+      <c r="G1" t="s">
+        <v>271</v>
+      </c>
+      <c r="H1" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" t="s">
+        <v>277</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="41">
+        <v>777</v>
+      </c>
+      <c r="B2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18.75">
+      <c r="A3">
+        <v>708</v>
+      </c>
+      <c r="B3" s="27">
+        <v>666</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A4">
+        <v>709</v>
+      </c>
+      <c r="B4" s="27">
+        <v>666</v>
+      </c>
+      <c r="H4" s="54" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75">
+      <c r="A5">
+        <v>710</v>
+      </c>
+      <c r="C5" s="26">
+        <v>123</v>
+      </c>
+      <c r="H5" s="54" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A6">
+        <v>710</v>
+      </c>
+      <c r="D6">
+        <v>5555</v>
+      </c>
+      <c r="H6" s="54" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A7" s="28">
+        <v>2000</v>
+      </c>
+      <c r="C7" s="26">
+        <v>200</v>
+      </c>
+      <c r="H7" s="54" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A8" s="28">
+        <v>2001</v>
+      </c>
+      <c r="C8" s="26">
+        <v>200</v>
+      </c>
+      <c r="H8" s="54" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" thickBot="1">
+      <c r="A9" s="28">
+        <v>2002</v>
+      </c>
+      <c r="C9" s="26">
+        <v>200</v>
+      </c>
+      <c r="H9" s="54" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18.75">
+      <c r="A10" s="28">
+        <v>2003</v>
+      </c>
+      <c r="C10" s="26">
+        <v>200</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>287</v>
+      </c>
+      <c r="K10" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1"/>
+    <row r="14" spans="1:12">
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="46"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="H15" s="49"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="C16" s="47"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48" t="s">
+        <v>273</v>
+      </c>
+      <c r="G16" s="48">
+        <v>1</v>
+      </c>
+      <c r="H16" s="49"/>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48" t="s">
+        <v>274</v>
+      </c>
+      <c r="G17" s="48">
+        <v>2</v>
+      </c>
+      <c r="H17" s="49"/>
+    </row>
+    <row r="18" spans="3:8">
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+    </row>
+    <row r="19" spans="3:8">
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+    </row>
+    <row r="20" spans="3:8">
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+    </row>
+    <row r="21" spans="3:8">
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
+    </row>
+    <row r="22" spans="3:8" ht="15" thickBot="1">
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="52"/>
+    </row>
+    <row r="25" spans="3:8" ht="15" thickBot="1"/>
+    <row r="26" spans="3:8">
+      <c r="C26" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D26" s="26">
+        <v>123</v>
+      </c>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="3:8">
+      <c r="C27" s="19"/>
+      <c r="D27" s="27" t="s">
+        <v>245</v>
+      </c>
+      <c r="E27" s="27">
+        <v>666</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+    </row>
+    <row r="28" spans="3:8">
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="F28" s="28">
+        <v>777</v>
+      </c>
+      <c r="G28" s="20"/>
+      <c r="H28" s="21" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8">
+      <c r="C29" s="19"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28">
+        <v>778</v>
+      </c>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
+      <c r="C30" s="19"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28">
+        <v>779</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8">
+      <c r="C31" s="19"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28">
+        <v>710</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="15" thickBot="1">
+      <c r="C32" s="22"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="35" spans="3:8" ht="15" thickBot="1"/>
+    <row r="36" spans="3:8">
+      <c r="C36" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="D36" s="26">
+        <v>123</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="18"/>
+    </row>
+    <row r="37" spans="3:8">
+      <c r="C37" s="19"/>
+      <c r="D37" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="E37" s="28">
+        <v>777</v>
+      </c>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="H37" s="21"/>
+    </row>
+    <row r="38" spans="3:8">
+      <c r="C38" s="19"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28">
+        <v>778</v>
+      </c>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
+      <c r="C39" s="19"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28">
+        <v>779</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G39" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
+      <c r="C40" s="19"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28">
+        <v>710</v>
+      </c>
+      <c r="F40" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="G40" s="21" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8">
+      <c r="C41" s="19"/>
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="3:8" ht="15" thickBot="1">
+      <c r="C42" s="22"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J24"/>
   <sheetViews>
@@ -1703,7 +3593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1904,7 +3794,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
@@ -2428,7 +4318,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2489,7 +4379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2547,7 +4437,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -2922,7 +4812,73 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor theme="9" tint="-0.249977111117893"/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -3007,7 +4963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -3054,7 +5010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
@@ -3132,7 +5088,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -3157,7 +5113,7 @@
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C1" s="10" t="s">
         <v>129</v>
@@ -3194,7 +5150,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -3222,28 +5178,28 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1" t="s">
         <v>197</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H1" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" t="s">
         <v>198</v>
-      </c>
-      <c r="D1" t="s">
-        <v>200</v>
-      </c>
-      <c r="E1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F1" t="s">
-        <v>202</v>
-      </c>
-      <c r="G1" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I1" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3251,7 +5207,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
@@ -3275,16 +5231,16 @@
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" t="s">
         <v>205</v>
-      </c>
-      <c r="C1" t="s">
-        <v>206</v>
       </c>
       <c r="D1" t="s">
         <v>192</v>
       </c>
       <c r="E1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3292,15 +5248,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3314,7 +5270,7 @@
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>2</v>
@@ -3326,72 +5282,21 @@
         <v>7</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="H1" s="43" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>235</v>
-      </c>
       <c r="I1" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <tabColor theme="6" tint="-0.249977111117893"/>
-  </sheetPr>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1">
-      <c r="A1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3400,92 +5305,84 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="9" customFormat="1">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:10" s="9" customFormat="1">
+      <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>215</v>
+        <v>2</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>217</v>
+        <v>7</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>218</v>
+        <v>109</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q1" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>229</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1"/>
+    <row r="10" spans="1:10" ht="15">
+      <c r="C10" s="37" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="H10" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29.25" thickBot="1">
+      <c r="C11" s="35"/>
+      <c r="D11" s="38" t="s">
+        <v>259</v>
+      </c>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="H12" s="33"/>
+      <c r="I12" s="34" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1">
+      <c r="H13" s="35"/>
+      <c r="I13" s="36" t="s">
+        <v>257</v>
       </c>
     </row>
   </sheetData>
@@ -3498,31 +5395,96 @@
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>231</v>
+        <v>253</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>252</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>230</v>
+        <v>212</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
infras - get names
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0001BAAD-C938-45DA-B32D-EE3B874DC36D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877720E3-BC59-438E-B15A-4A42ED1DDB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1768,7 +1768,9 @@
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
added Process class with api - before test
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877720E3-BC59-438E-B15A-4A42ED1DDB2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="929" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" tabRatio="929" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="21" r:id="rId1"/>
@@ -30,7 +29,7 @@
     <sheet name="Trees" sheetId="8" r:id="rId20"/>
     <sheet name="Groups" sheetId="9" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="302">
   <si>
     <t>callback</t>
   </si>
@@ -250,18 +249,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
   </si>
   <si>
     <t>users</t>
@@ -1081,16 +1068,19 @@
   <si>
     <t>filter - json project:, owner:,tags:</t>
   </si>
+  <si>
+    <t>owner_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1115,7 +1105,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1443,7 +1433,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1485,7 +1475,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1517,27 +1507,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1569,24 +1541,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1762,67 +1716,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="56" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="57" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="57" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="57" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="57" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="57" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
       <c r="A5" s="57" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
       <c r="A6" s="57" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
       <c r="A7" s="57"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" s="57" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
       <c r="A9" s="57" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15" thickBot="1">
       <c r="A10" s="58" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -1831,7 +1785,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1841,25 +1795,25 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1868,7 +1822,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1878,52 +1832,52 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18.75">
       <c r="A2" s="13">
         <v>123</v>
       </c>
@@ -1937,10 +1891,10 @@
         <v>0</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="19.5" thickBot="1">
       <c r="A3">
         <v>333</v>
       </c>
@@ -1954,10 +1908,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="54" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="26">
         <v>200</v>
       </c>
@@ -1971,53 +1925,53 @@
         <v>0</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75">
       <c r="H5" s="54" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18.75">
       <c r="H6" s="54" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18.75">
       <c r="H7" s="54" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
       <c r="F8" s="54"/>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="C9" s="31" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F9" s="54"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="15" thickBot="1">
       <c r="C10" s="42" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="C11" s="55"/>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="15" thickBot="1">
       <c r="C12" s="55"/>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -2025,50 +1979,50 @@
       <c r="G13" s="45"/>
       <c r="H13" s="46"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="C14" s="47"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
       <c r="F14" s="48"/>
       <c r="G14" s="48" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="H14" s="49"/>
       <c r="J14" s="13" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
       <c r="F15" s="48" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="G15" s="48">
         <v>1</v>
       </c>
       <c r="H15" s="49"/>
       <c r="K15" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G16" s="48">
         <v>2</v>
       </c>
       <c r="H16" s="49"/>
       <c r="L16" s="16" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
@@ -2077,7 +2031,7 @@
       <c r="H17" s="49"/>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -2086,7 +2040,7 @@
       <c r="H18" s="49"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -2094,7 +2048,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -2102,7 +2056,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:12" ht="15" thickBot="1">
       <c r="C21" s="50"/>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
@@ -2110,27 +2064,27 @@
       <c r="G21" s="51"/>
       <c r="H21" s="52"/>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:12">
       <c r="C22" s="55"/>
       <c r="D22" s="20"/>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12">
       <c r="C23" s="55"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12">
       <c r="C24" s="55"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12" ht="15">
       <c r="I25" s="30" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" ht="15" thickBot="1"/>
+    <row r="27" spans="3:12">
       <c r="C27" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D27" s="26">
         <v>123</v>
@@ -2140,10 +2094,10 @@
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:12">
       <c r="C28" s="19"/>
       <c r="D28" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E28" s="27">
         <v>666</v>
@@ -2152,21 +2106,21 @@
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:12">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F29" s="28">
         <v>777</v>
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="3:12">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2175,10 +2129,10 @@
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="3:12">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -2186,13 +2140,13 @@
         <v>779</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="3:12">
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="28"/>
@@ -2200,13 +2154,13 @@
         <v>710</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H32" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="33" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="15" thickBot="1">
       <c r="C33" s="22"/>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -2214,15 +2168,15 @@
       <c r="G33" s="23"/>
       <c r="H33" s="24"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" ht="15">
       <c r="I35" s="30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" ht="15" thickBot="1"/>
+    <row r="37" spans="3:9">
       <c r="C37" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D37" s="26">
         <v>333</v>
@@ -2232,10 +2186,10 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9">
       <c r="C38" s="19"/>
       <c r="D38" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E38" s="27">
         <v>680</v>
@@ -2244,21 +2198,21 @@
       <c r="G38" s="20"/>
       <c r="H38" s="21"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9">
       <c r="C39" s="19"/>
       <c r="D39" s="20"/>
       <c r="E39" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F39" s="28">
         <v>800</v>
       </c>
       <c r="G39" s="20"/>
       <c r="H39" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9">
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
       <c r="E40" s="28"/>
@@ -2267,10 +2221,10 @@
       </c>
       <c r="G40" s="20"/>
       <c r="H40" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
       <c r="E41" s="28"/>
@@ -2278,13 +2232,13 @@
         <v>802</v>
       </c>
       <c r="G41" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9">
       <c r="C42" s="19"/>
       <c r="D42" s="20"/>
       <c r="E42" s="28"/>
@@ -2292,16 +2246,16 @@
         <v>803</v>
       </c>
       <c r="G42" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9">
       <c r="C43" s="19"/>
       <c r="D43" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E43" s="27">
         <v>681</v>
@@ -2310,21 +2264,21 @@
       <c r="G43" s="20"/>
       <c r="H43" s="21"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9">
       <c r="C44" s="19"/>
       <c r="D44" s="20"/>
       <c r="E44" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F44" s="28">
         <v>803</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9">
       <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="28"/>
@@ -2333,10 +2287,10 @@
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9">
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="28"/>
@@ -2344,13 +2298,13 @@
         <v>805</v>
       </c>
       <c r="G46" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H46" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" ht="15" thickBot="1">
       <c r="C47" s="22"/>
       <c r="D47" s="23"/>
       <c r="E47" s="29"/>
@@ -2358,20 +2312,20 @@
         <v>806</v>
       </c>
       <c r="G47" s="23" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H47" s="24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" ht="15" thickBot="1">
+      <c r="I51" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9">
+      <c r="C52" s="25" t="s">
         <v>240</v>
-      </c>
-    </row>
-    <row r="51" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I51" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
-      <c r="C52" s="25" t="s">
-        <v>244</v>
       </c>
       <c r="D52" s="26">
         <v>444</v>
@@ -2381,10 +2335,10 @@
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9">
       <c r="C53" s="19"/>
       <c r="D53" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E53" s="27">
         <v>900</v>
@@ -2393,21 +2347,21 @@
       <c r="G53" s="20"/>
       <c r="H53" s="21"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9">
       <c r="C54" s="19"/>
       <c r="D54" s="20"/>
       <c r="E54" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F54" s="28">
         <v>1001</v>
       </c>
       <c r="G54" s="20"/>
       <c r="H54" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9">
       <c r="C55" s="19"/>
       <c r="D55" s="20"/>
       <c r="E55" s="28"/>
@@ -2416,13 +2370,13 @@
       </c>
       <c r="G55" s="20"/>
       <c r="H55" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9">
       <c r="C56" s="19"/>
       <c r="D56" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E56" s="27">
         <v>901</v>
@@ -2431,21 +2385,21 @@
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9">
       <c r="C57" s="19"/>
       <c r="D57" s="20"/>
       <c r="E57" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F57" s="28">
         <v>1003</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" ht="15" thickBot="1">
       <c r="C58" s="22"/>
       <c r="D58" s="23"/>
       <c r="E58" s="29"/>
@@ -2454,13 +2408,13 @@
       </c>
       <c r="G58" s="23"/>
       <c r="H58" s="24" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="63" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="3:9" ht="15" thickBot="1"/>
+    <row r="64" spans="3:9">
       <c r="C64" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D64" s="26">
         <v>200</v>
@@ -2470,21 +2424,21 @@
       <c r="G64" s="17"/>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:8">
       <c r="C65" s="19"/>
       <c r="D65" s="20"/>
       <c r="E65" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F65" s="28">
         <v>2000</v>
       </c>
       <c r="G65" s="20"/>
       <c r="H65" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8">
       <c r="C66" s="19"/>
       <c r="D66" s="20"/>
       <c r="E66" s="28"/>
@@ -2493,10 +2447,10 @@
       </c>
       <c r="G66" s="20"/>
       <c r="H66" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8">
       <c r="C67" s="19"/>
       <c r="D67" s="20"/>
       <c r="E67" s="28"/>
@@ -2504,13 +2458,13 @@
         <v>2002</v>
       </c>
       <c r="G67" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="68" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" ht="15" thickBot="1">
       <c r="C68" s="22"/>
       <c r="D68" s="23"/>
       <c r="E68" s="29"/>
@@ -2518,10 +2472,10 @@
         <v>2003</v>
       </c>
       <c r="G68" s="23" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H68" s="24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2531,7 +2485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2541,48 +2495,48 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D1" s="40" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="27">
         <v>666</v>
       </c>
@@ -2591,18 +2545,18 @@
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="41" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15">
       <c r="I9" s="30" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickBot="1"/>
+    <row r="11" spans="1:9">
       <c r="C11" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D11" s="26">
         <v>123</v>
@@ -2612,10 +2566,10 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="C12" s="19"/>
       <c r="D12" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E12" s="27">
         <v>666</v>
@@ -2624,21 +2578,21 @@
       <c r="G12" s="20"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F13" s="28">
         <v>777</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="28"/>
@@ -2647,10 +2601,10 @@
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="28"/>
@@ -2658,13 +2612,13 @@
         <v>779</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="28"/>
@@ -2672,13 +2626,13 @@
         <v>710</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="17" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" ht="15" thickBot="1">
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2686,15 +2640,15 @@
       <c r="G17" s="23"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" ht="15">
       <c r="I19" s="30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="20" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" ht="15" thickBot="1"/>
+    <row r="21" spans="3:9">
       <c r="C21" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D21" s="26">
         <v>333</v>
@@ -2704,10 +2658,10 @@
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9">
       <c r="C22" s="19"/>
       <c r="D22" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E22" s="27">
         <v>680</v>
@@ -2716,21 +2670,21 @@
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9">
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F23" s="28">
         <v>800</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9">
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="28"/>
@@ -2739,10 +2693,10 @@
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9">
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
@@ -2750,13 +2704,13 @@
         <v>802</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H25" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9">
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
       <c r="E26" s="28"/>
@@ -2764,16 +2718,16 @@
         <v>803</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E27" s="27">
         <v>681</v>
@@ -2782,21 +2736,21 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:9">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F28" s="28">
         <v>803</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -2805,10 +2759,10 @@
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2816,13 +2770,13 @@
         <v>805</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" ht="15" thickBot="1">
       <c r="C31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="29"/>
@@ -2830,10 +2784,10 @@
         <v>806</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2843,7 +2797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2853,67 +2807,67 @@
       <selection activeCell="H3" sqref="H3:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
     <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C1" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="H1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="41">
         <v>777</v>
       </c>
       <c r="B2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3">
         <v>708</v>
       </c>
@@ -2921,10 +2875,10 @@
         <v>666</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="19.5" thickBot="1">
       <c r="A4">
         <v>709</v>
       </c>
@@ -2932,10 +2886,10 @@
         <v>666</v>
       </c>
       <c r="H4" s="54" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5">
         <v>710</v>
       </c>
@@ -2943,10 +2897,10 @@
         <v>123</v>
       </c>
       <c r="H5" s="54" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="19.5" thickBot="1">
       <c r="A6">
         <v>710</v>
       </c>
@@ -2954,10 +2908,10 @@
         <v>5555</v>
       </c>
       <c r="H6" s="54" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="19.5" thickBot="1">
       <c r="A7" s="28">
         <v>2000</v>
       </c>
@@ -2965,10 +2919,10 @@
         <v>200</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
       <c r="A8" s="28">
         <v>2001</v>
       </c>
@@ -2976,10 +2930,10 @@
         <v>200</v>
       </c>
       <c r="H8" s="54" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="19.5" thickBot="1">
       <c r="A9" s="28">
         <v>2002</v>
       </c>
@@ -2987,10 +2941,10 @@
         <v>200</v>
       </c>
       <c r="H9" s="54" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18.75">
       <c r="A10" s="28">
         <v>2003</v>
       </c>
@@ -2998,14 +2952,14 @@
         <v>200</v>
       </c>
       <c r="H10" s="54" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="K10" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15" thickBot="1"/>
+    <row r="14" spans="1:12">
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -3013,41 +2967,41 @@
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
       <c r="F15" s="48"/>
       <c r="G15" s="48" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="H15" s="49"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
       <c r="F16" s="48" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="G16" s="48">
         <v>1</v>
       </c>
       <c r="H16" s="49"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:8">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
       <c r="F17" s="48" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G17" s="48">
         <v>2</v>
       </c>
       <c r="H17" s="49"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:8">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -3055,7 +3009,7 @@
       <c r="G18" s="48"/>
       <c r="H18" s="49"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:8">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -3063,7 +3017,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:8">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -3071,7 +3025,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:8">
       <c r="C21" s="47"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
@@ -3079,7 +3033,7 @@
       <c r="G21" s="48"/>
       <c r="H21" s="49"/>
     </row>
-    <row r="22" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:8" ht="15" thickBot="1">
       <c r="C22" s="50"/>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
@@ -3087,10 +3041,10 @@
       <c r="G22" s="51"/>
       <c r="H22" s="52"/>
     </row>
-    <row r="25" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:8" ht="15" thickBot="1"/>
+    <row r="26" spans="3:8">
       <c r="C26" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D26" s="26">
         <v>123</v>
@@ -3100,10 +3054,10 @@
       <c r="G26" s="17"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:8">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E27" s="27">
         <v>666</v>
@@ -3112,21 +3066,21 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:8">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F28" s="28">
         <v>777</v>
       </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="29" spans="3:8">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -3135,10 +3089,10 @@
       </c>
       <c r="G29" s="20"/>
       <c r="H29" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -3146,13 +3100,13 @@
         <v>779</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H30" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="3:8">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -3160,13 +3114,13 @@
         <v>710</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H31" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="15" thickBot="1">
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -3174,10 +3128,10 @@
       <c r="G32" s="23"/>
       <c r="H32" s="24"/>
     </row>
-    <row r="35" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:8" ht="15" thickBot="1"/>
+    <row r="36" spans="3:8">
       <c r="C36" s="25" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D36" s="26">
         <v>123</v>
@@ -3187,21 +3141,21 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8">
       <c r="C37" s="19"/>
       <c r="D37" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E37" s="28">
         <v>777</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="21" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8">
       <c r="C38" s="19"/>
       <c r="D38" s="28"/>
       <c r="E38" s="28">
@@ -3209,40 +3163,40 @@
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="21" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="3:8">
       <c r="C39" s="19"/>
       <c r="D39" s="28"/>
       <c r="E39" s="28">
         <v>779</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G39" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="40" spans="3:8">
       <c r="C40" s="19"/>
       <c r="D40" s="28"/>
       <c r="E40" s="28">
         <v>710</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G40" s="21" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="41" spans="3:8">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
     </row>
-    <row r="42" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="3:8" ht="15" thickBot="1">
       <c r="C42" s="22"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -3257,28 +3211,28 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3289,28 +3243,28 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" t="s">
         <v>79</v>
       </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>81</v>
-      </c>
-      <c r="I1" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3336,13 +3290,13 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3365,16 +3319,16 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3397,16 +3351,16 @@
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3429,16 +3383,16 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3464,13 +3418,13 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3493,16 +3447,16 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3525,16 +3479,16 @@
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3557,43 +3511,43 @@
         <v>8</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" ht="15">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" ht="15">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" ht="15">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" ht="15">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" ht="15">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" ht="15">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" ht="15">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" ht="15">
       <c r="C24" s="3"/>
     </row>
   </sheetData>
@@ -3603,43 +3557,43 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -3648,16 +3602,16 @@
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E2" s="4">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -3666,16 +3620,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E3" s="4">
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>2</v>
@@ -3684,16 +3638,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E4" s="4">
         <v>4</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -3702,16 +3656,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -3720,16 +3674,16 @@
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
@@ -3738,16 +3692,16 @@
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E7" s="4">
         <v>66</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" s="4">
         <v>2</v>
       </c>
@@ -3755,16 +3709,16 @@
         <v>2</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9" s="4">
         <v>3</v>
       </c>
@@ -3772,16 +3726,16 @@
         <v>2</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -3789,13 +3743,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -3804,32 +3758,32 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.36328125" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.375" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3840,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -3882,13 +3836,13 @@
         <v>53</v>
       </c>
       <c r="R1" s="5" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3896,13 +3850,13 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3941,10 +3895,10 @@
         <v>1</v>
       </c>
       <c r="S2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3952,13 +3906,13 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F3">
         <v>2</v>
@@ -3997,10 +3951,10 @@
         <v>1</v>
       </c>
       <c r="S3" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4008,13 +3962,13 @@
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F4">
         <v>3</v>
@@ -4054,7 +4008,7 @@
       </c>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4062,13 +4016,13 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -4107,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4115,13 +4069,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -4160,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4168,13 +4122,13 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -4213,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4221,10 +4175,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E8" t="str">
         <f>CONCATENATE("c:/functions/",C8)</f>
@@ -4267,7 +4221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4278,7 +4232,7 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E9" t="str">
         <f>CONCATENATE("c:/functions/",C9)</f>
@@ -4306,7 +4260,7 @@
         <v>7</v>
       </c>
       <c r="N9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="O9" t="s">
         <v>36</v>
@@ -4328,59 +4282,59 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -4389,56 +4343,56 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -4447,56 +4401,56 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D1" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
         <v>134</v>
-      </c>
-      <c r="E1" t="s">
-        <v>137</v>
-      </c>
-      <c r="F1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E2" t="s">
-        <v>138</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4510,13 +4464,13 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4527,16 +4481,16 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4547,16 +4501,16 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4570,13 +4524,13 @@
         <v>26</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4587,16 +4541,16 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4607,16 +4561,16 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4627,16 +4581,16 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4647,16 +4601,16 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4667,16 +4621,16 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4687,16 +4641,16 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4707,16 +4661,16 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E13" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4730,13 +4684,13 @@
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4747,16 +4701,16 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4767,16 +4721,16 @@
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4790,13 +4744,13 @@
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4807,10 +4761,10 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E18" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -4822,23 +4776,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4849,16 +4803,16 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4871,7 +4825,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4884,7 +4838,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4897,7 +4851,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4909,58 +4863,6 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4968,35 +4870,35 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5005,12 +4907,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -5019,12 +4921,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -5033,12 +4935,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -5053,45 +4955,45 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -5100,7 +5002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5110,66 +5012,66 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D1" t="s">
         <v>43</v>
       </c>
       <c r="E1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G1" t="s">
+        <v>182</v>
+      </c>
+      <c r="H1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I1" t="s">
         <v>180</v>
       </c>
-      <c r="F1" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>179</v>
+      </c>
+      <c r="K1" t="s">
+        <v>178</v>
+      </c>
+      <c r="L1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N1" t="s">
         <v>186</v>
       </c>
-      <c r="H1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" t="s">
-        <v>184</v>
-      </c>
-      <c r="J1" t="s">
-        <v>183</v>
-      </c>
-      <c r="K1" t="s">
-        <v>182</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>187</v>
-      </c>
-      <c r="M1" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" t="s">
-        <v>190</v>
-      </c>
-      <c r="O1" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -5178,7 +5080,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5188,24 +5090,24 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="11" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>2</v>
@@ -5217,16 +5119,16 @@
         <v>7</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H1" s="10" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -5240,7 +5142,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5250,45 +5152,45 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" t="s">
         <v>196</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>197</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" t="s">
         <v>199</v>
       </c>
-      <c r="E1" t="s">
-        <v>200</v>
-      </c>
-      <c r="F1" t="s">
-        <v>201</v>
-      </c>
-      <c r="G1" t="s">
-        <v>202</v>
-      </c>
-      <c r="H1" t="s">
-        <v>203</v>
-      </c>
       <c r="I1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5297,7 +5199,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5307,29 +5209,29 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -5338,31 +5240,31 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="9" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>2</v>
+        <v>301</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>6</v>
@@ -5371,17 +5273,44 @@
         <v>7</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H1" s="43" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>209</v>
-      </c>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="D10" s="9"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="D11" s="9"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="D12" s="9"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="D14" s="9"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="D16" s="43"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5390,35 +5319,37 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="9" customFormat="1">
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>2</v>
@@ -5430,48 +5361,48 @@
         <v>7</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1"/>
+    <row r="10" spans="1:10" ht="15">
       <c r="C10" s="37" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D10" s="32"/>
       <c r="H10" s="37" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="I10" s="32" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="29.25" thickBot="1">
       <c r="C11" s="35"/>
       <c r="D11" s="38" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H11" s="33"/>
       <c r="I11" s="34" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="H12" s="33"/>
       <c r="I12" s="34" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="H13" s="35"/>
       <c r="I13" s="36" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -5480,7 +5411,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5490,90 +5421,90 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C1" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="M1" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="N1" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="O1" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="P1" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="M1" s="9" t="s">
+      <c r="R1" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="N1" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="O1" s="9" t="s">
+      <c r="S1" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>223</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ComplexNet, NetConfig and NetSystem backend done in model
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A040CD2-0432-4C2C-B97F-C5B6BDE2007D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="10200" tabRatio="929" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="10200" tabRatio="929" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="21" r:id="rId1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="348">
   <si>
     <t>callback</t>
   </si>
@@ -1183,7 +1182,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1193,7 +1192,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1237,12 +1236,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1267,7 +1266,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1596,7 +1595,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1638,7 +1637,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1670,27 +1669,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1722,24 +1703,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1915,7 +1878,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1925,55 +1888,55 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1">
       <c r="A1" s="56" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1">
       <c r="A2" s="57" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1">
       <c r="A3" s="57" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1">
       <c r="A4" s="57" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1">
       <c r="A5" s="57" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1">
       <c r="A6" s="57" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1">
       <c r="A7" s="57"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1">
       <c r="A8" s="57" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1">
       <c r="A9" s="57" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:1" ht="15" thickBot="1">
       <c r="A10" s="58" t="s">
         <v>295</v>
       </c>
@@ -1984,7 +1947,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1994,14 +1957,14 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -2021,7 +1984,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2031,20 +1994,20 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.08984375" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.125" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>240</v>
       </c>
@@ -2076,7 +2039,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:12" ht="18.75">
       <c r="A2" s="13">
         <v>123</v>
       </c>
@@ -2093,7 +2056,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" ht="19.5" thickBot="1">
       <c r="A3">
         <v>333</v>
       </c>
@@ -2110,7 +2073,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:12" ht="18.75">
       <c r="A4" s="26">
         <v>200</v>
       </c>
@@ -2127,25 +2090,25 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="H5" s="54" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:12" ht="18.75">
       <c r="H6" s="54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:12" ht="18.75">
       <c r="H7" s="54" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
       <c r="F8" s="54"/>
     </row>
-    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:12" ht="18.75">
       <c r="C9" s="31" t="s">
         <v>261</v>
       </c>
@@ -2154,7 +2117,7 @@
       </c>
       <c r="F9" s="54"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="15" thickBot="1">
       <c r="C10" s="42" t="s">
         <v>262</v>
       </c>
@@ -2162,15 +2125,15 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="C11" s="55"/>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:12" ht="15" thickBot="1">
       <c r="C12" s="55"/>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -2178,7 +2141,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="46"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="C14" s="47"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
@@ -2191,7 +2154,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -2206,7 +2169,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
@@ -2221,7 +2184,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:12">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
@@ -2230,7 +2193,7 @@
       <c r="H17" s="49"/>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:12">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -2239,7 +2202,7 @@
       <c r="H18" s="49"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:12">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -2247,7 +2210,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:12">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -2255,7 +2218,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:12" ht="15" thickBot="1">
       <c r="C21" s="50"/>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
@@ -2263,25 +2226,25 @@
       <c r="G21" s="51"/>
       <c r="H21" s="52"/>
     </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:12">
       <c r="C22" s="55"/>
       <c r="D22" s="20"/>
     </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:12">
       <c r="C23" s="55"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:12">
       <c r="C24" s="55"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:12" ht="15">
       <c r="I25" s="30" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:12" ht="15" thickBot="1"/>
+    <row r="27" spans="3:12">
       <c r="C27" s="25" t="s">
         <v>240</v>
       </c>
@@ -2293,7 +2256,7 @@
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:12">
       <c r="C28" s="19"/>
       <c r="D28" s="27" t="s">
         <v>241</v>
@@ -2305,7 +2268,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:12">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28" t="s">
@@ -2319,7 +2282,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:12">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2331,7 +2294,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:12">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -2345,7 +2308,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:12">
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="28"/>
@@ -2359,7 +2322,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="3:9" ht="15" thickBot="1">
       <c r="C33" s="22"/>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -2367,13 +2330,13 @@
       <c r="G33" s="23"/>
       <c r="H33" s="24"/>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:9" ht="15">
       <c r="I35" s="30" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:9" ht="15" thickBot="1"/>
+    <row r="37" spans="3:9">
       <c r="C37" s="25" t="s">
         <v>240</v>
       </c>
@@ -2385,7 +2348,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:9">
       <c r="C38" s="19"/>
       <c r="D38" s="27" t="s">
         <v>241</v>
@@ -2397,7 +2360,7 @@
       <c r="G38" s="20"/>
       <c r="H38" s="21"/>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:9">
       <c r="C39" s="19"/>
       <c r="D39" s="20"/>
       <c r="E39" s="28" t="s">
@@ -2411,7 +2374,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:9">
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
       <c r="E40" s="28"/>
@@ -2423,7 +2386,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:9">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
       <c r="E41" s="28"/>
@@ -2437,7 +2400,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:9">
       <c r="C42" s="19"/>
       <c r="D42" s="20"/>
       <c r="E42" s="28"/>
@@ -2451,7 +2414,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:9">
       <c r="C43" s="19"/>
       <c r="D43" s="27" t="s">
         <v>241</v>
@@ -2463,7 +2426,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="21"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:9">
       <c r="C44" s="19"/>
       <c r="D44" s="20"/>
       <c r="E44" s="28" t="s">
@@ -2477,7 +2440,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:9">
       <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="28"/>
@@ -2489,7 +2452,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:9">
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="28"/>
@@ -2503,7 +2466,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="3:9" ht="15" thickBot="1">
       <c r="C47" s="22"/>
       <c r="D47" s="23"/>
       <c r="E47" s="29"/>
@@ -2517,12 +2480,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="3:9" ht="15" thickBot="1">
       <c r="I51" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:9">
       <c r="C52" s="25" t="s">
         <v>240</v>
       </c>
@@ -2534,7 +2497,7 @@
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:9">
       <c r="C53" s="19"/>
       <c r="D53" s="27" t="s">
         <v>241</v>
@@ -2546,7 +2509,7 @@
       <c r="G53" s="20"/>
       <c r="H53" s="21"/>
     </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:9">
       <c r="C54" s="19"/>
       <c r="D54" s="20"/>
       <c r="E54" s="28" t="s">
@@ -2560,7 +2523,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:9">
       <c r="C55" s="19"/>
       <c r="D55" s="20"/>
       <c r="E55" s="28"/>
@@ -2572,7 +2535,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:9">
       <c r="C56" s="19"/>
       <c r="D56" s="27" t="s">
         <v>241</v>
@@ -2584,7 +2547,7 @@
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
     </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:9">
       <c r="C57" s="19"/>
       <c r="D57" s="20"/>
       <c r="E57" s="28" t="s">
@@ -2598,7 +2561,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="3:9" ht="15" thickBot="1">
       <c r="C58" s="22"/>
       <c r="D58" s="23"/>
       <c r="E58" s="29"/>
@@ -2610,8 +2573,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="64" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:9" ht="15" thickBot="1"/>
+    <row r="64" spans="3:9">
       <c r="C64" s="25" t="s">
         <v>240</v>
       </c>
@@ -2623,7 +2586,7 @@
       <c r="G64" s="17"/>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="3:8">
       <c r="C65" s="19"/>
       <c r="D65" s="20"/>
       <c r="E65" s="28" t="s">
@@ -2637,7 +2600,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="3:8">
       <c r="C66" s="19"/>
       <c r="D66" s="20"/>
       <c r="E66" s="28"/>
@@ -2649,7 +2612,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="3:8">
       <c r="C67" s="19"/>
       <c r="D67" s="20"/>
       <c r="E67" s="28"/>
@@ -2663,7 +2626,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="3:8" ht="15" thickBot="1">
       <c r="C68" s="22"/>
       <c r="D68" s="23"/>
       <c r="E68" s="29"/>
@@ -2684,7 +2647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2694,19 +2657,19 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -2735,7 +2698,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="27">
         <v>666</v>
       </c>
@@ -2747,13 +2710,13 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="15">
       <c r="I9" s="30" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="15" thickBot="1"/>
+    <row r="11" spans="1:9">
       <c r="C11" s="25" t="s">
         <v>240</v>
       </c>
@@ -2765,7 +2728,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="C12" s="19"/>
       <c r="D12" s="27" t="s">
         <v>241</v>
@@ -2777,7 +2740,7 @@
       <c r="G12" s="20"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="28" t="s">
@@ -2791,7 +2754,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="28"/>
@@ -2803,7 +2766,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="28"/>
@@ -2817,7 +2780,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="28"/>
@@ -2831,7 +2794,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="3:9" ht="15" thickBot="1">
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2839,13 +2802,13 @@
       <c r="G17" s="23"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" ht="15">
       <c r="I19" s="30" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:9" ht="15" thickBot="1"/>
+    <row r="21" spans="3:9">
       <c r="C21" s="25" t="s">
         <v>240</v>
       </c>
@@ -2857,7 +2820,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:9">
       <c r="C22" s="19"/>
       <c r="D22" s="27" t="s">
         <v>241</v>
@@ -2869,7 +2832,7 @@
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:9">
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="28" t="s">
@@ -2883,7 +2846,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:9">
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="28"/>
@@ -2895,7 +2858,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:9">
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
@@ -2909,7 +2872,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:9">
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
       <c r="E26" s="28"/>
@@ -2923,7 +2886,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:9">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
         <v>241</v>
@@ -2935,7 +2898,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:9">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
@@ -2949,7 +2912,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:9">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -2961,7 +2924,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:9">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2975,7 +2938,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="3:9" ht="15" thickBot="1">
       <c r="C31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="29"/>
@@ -2996,7 +2959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -3006,21 +2969,21 @@
       <selection activeCell="H3" sqref="H3:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.625" customWidth="1"/>
     <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3058,7 +3021,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="41">
         <v>777</v>
       </c>
@@ -3066,7 +3029,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:12" ht="18.75">
       <c r="A3">
         <v>708</v>
       </c>
@@ -3077,7 +3040,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" ht="19.5" thickBot="1">
       <c r="A4">
         <v>709</v>
       </c>
@@ -3088,7 +3051,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:12" ht="18.75">
       <c r="A5">
         <v>710</v>
       </c>
@@ -3099,7 +3062,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" ht="19.5" thickBot="1">
       <c r="A6">
         <v>710</v>
       </c>
@@ -3110,7 +3073,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" ht="19.5" thickBot="1">
       <c r="A7" s="28">
         <v>2000</v>
       </c>
@@ -3121,7 +3084,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" ht="19.5" thickBot="1">
       <c r="A8" s="28">
         <v>2001</v>
       </c>
@@ -3132,7 +3095,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="19.5" thickBot="1">
       <c r="A9" s="28">
         <v>2002</v>
       </c>
@@ -3143,7 +3106,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:12" ht="18.75">
       <c r="A10" s="28">
         <v>2003</v>
       </c>
@@ -3157,8 +3120,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" ht="15" thickBot="1"/>
+    <row r="14" spans="1:12">
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -3166,7 +3129,7 @@
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -3176,7 +3139,7 @@
       </c>
       <c r="H15" s="49"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
@@ -3188,7 +3151,7 @@
       </c>
       <c r="H16" s="49"/>
     </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:8">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
@@ -3200,7 +3163,7 @@
       </c>
       <c r="H17" s="49"/>
     </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:8">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -3208,7 +3171,7 @@
       <c r="G18" s="48"/>
       <c r="H18" s="49"/>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:8">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -3216,7 +3179,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:8">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -3224,7 +3187,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:8">
       <c r="C21" s="47"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
@@ -3232,7 +3195,7 @@
       <c r="G21" s="48"/>
       <c r="H21" s="49"/>
     </row>
-    <row r="22" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:8" ht="15" thickBot="1">
       <c r="C22" s="50"/>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
@@ -3240,8 +3203,8 @@
       <c r="G22" s="51"/>
       <c r="H22" s="52"/>
     </row>
-    <row r="25" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:8" ht="15" thickBot="1"/>
+    <row r="26" spans="3:8">
       <c r="C26" s="25" t="s">
         <v>240</v>
       </c>
@@ -3253,7 +3216,7 @@
       <c r="G26" s="17"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:8">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
         <v>241</v>
@@ -3265,7 +3228,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:8">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
@@ -3279,7 +3242,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:8">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -3291,7 +3254,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:8">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -3305,7 +3268,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:8">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -3319,7 +3282,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="3:8" ht="15" thickBot="1">
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -3327,8 +3290,8 @@
       <c r="G32" s="23"/>
       <c r="H32" s="24"/>
     </row>
-    <row r="35" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:8" ht="15" thickBot="1"/>
+    <row r="36" spans="3:8">
       <c r="C36" s="25" t="s">
         <v>240</v>
       </c>
@@ -3340,7 +3303,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8">
       <c r="C37" s="19"/>
       <c r="D37" s="28" t="s">
         <v>242</v>
@@ -3354,7 +3317,7 @@
       </c>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8">
       <c r="C38" s="19"/>
       <c r="D38" s="28"/>
       <c r="E38" s="28">
@@ -3365,7 +3328,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:8">
       <c r="C39" s="19"/>
       <c r="D39" s="28"/>
       <c r="E39" s="28">
@@ -3378,7 +3341,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:8">
       <c r="C40" s="19"/>
       <c r="D40" s="28"/>
       <c r="E40" s="28">
@@ -3391,11 +3354,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:8">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
     </row>
-    <row r="42" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="3:8" ht="15" thickBot="1">
       <c r="C42" s="22"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -3410,28 +3373,28 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3463,7 +3426,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3495,7 +3458,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3527,7 +3490,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3559,7 +3522,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3591,7 +3554,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3623,7 +3586,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3655,7 +3618,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3687,7 +3650,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3719,34 +3682,34 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="15">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" ht="15">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" ht="15">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" ht="15">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:3" ht="15">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:3" ht="15">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:3" ht="15">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:3" ht="15">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:3" ht="15">
       <c r="C24" s="3"/>
     </row>
   </sheetData>
@@ -3756,23 +3719,23 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.90625" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.75" customWidth="1"/>
+    <col min="5" max="5" width="15.875" customWidth="1"/>
+    <col min="6" max="6" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -3792,7 +3755,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -3810,7 +3773,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -3828,7 +3791,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>2</v>
@@ -3846,7 +3809,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -3864,7 +3827,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -3882,7 +3845,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
@@ -3900,7 +3863,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="B8" s="4">
         <v>2</v>
       </c>
@@ -3917,7 +3880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="B9" s="4">
         <v>3</v>
       </c>
@@ -3934,7 +3897,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -3957,32 +3920,32 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.36328125" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.375" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4041,7 +4004,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4097,7 +4060,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4153,7 +4116,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4207,7 +4170,7 @@
       </c>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4260,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4313,7 +4276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4366,7 +4329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4420,7 +4383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4481,19 +4444,19 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4504,7 +4467,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4512,7 +4475,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4520,7 +4483,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4528,7 +4491,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4542,16 +4505,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4562,7 +4525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4570,7 +4533,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4578,7 +4541,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4586,7 +4549,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4600,16 +4563,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4629,7 +4592,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4649,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4669,7 +4632,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4689,7 +4652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4709,7 +4672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4729,7 +4692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4749,7 +4712,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4769,7 +4732,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4789,7 +4752,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4809,7 +4772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4829,7 +4792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4849,7 +4812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4869,7 +4832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4889,7 +4852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4909,7 +4872,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4929,7 +4892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4949,7 +4912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4975,26 +4938,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.7265625" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5014,7 +4977,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5027,7 +4990,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5040,7 +5003,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5053,7 +5016,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5066,22 +5029,22 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10">
       <c r="G7" s="13" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10">
       <c r="H8" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10">
       <c r="I9" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="H12" t="s">
         <v>307</v>
       </c>
@@ -5089,65 +5052,65 @@
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10">
       <c r="J13" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10">
       <c r="J14" s="8" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10">
       <c r="J15" s="8" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10">
       <c r="J16" s="8" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:10">
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:10">
       <c r="I18" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:10">
       <c r="J19" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:10">
       <c r="J20" s="8" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="9:10">
       <c r="J21" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="9:10">
       <c r="J22" s="8" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="9:10">
       <c r="I23" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="9:10">
       <c r="J24" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="9:10">
       <c r="I26" t="s">
         <v>328</v>
       </c>
@@ -5155,32 +5118,32 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="9:10">
       <c r="J27" s="8" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="9:10">
       <c r="J28" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="9:10">
       <c r="J29" s="8" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="9:10">
       <c r="J30" s="8" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="9:10">
       <c r="J31" s="8" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:10">
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
@@ -5194,72 +5157,72 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:10">
       <c r="J34" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:10">
       <c r="J35" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:10">
       <c r="J36" s="8" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:10">
       <c r="I38" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:10">
       <c r="J39" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:10">
       <c r="J40" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:10">
       <c r="J41" s="8" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:10">
       <c r="J42" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:10">
       <c r="J43" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:10" ht="15">
       <c r="J44" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:10">
       <c r="I46" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:10">
       <c r="J47" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:10">
       <c r="J48" s="8" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="9:10">
       <c r="I50" t="s">
         <v>119</v>
       </c>
@@ -5267,22 +5230,22 @@
         <v>338</v>
       </c>
     </row>
-    <row r="51" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="9:10">
       <c r="J51" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="9:10">
       <c r="J52" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="9:10">
       <c r="J53" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="55" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="9:10">
       <c r="I55" t="s">
         <v>342</v>
       </c>
@@ -5290,12 +5253,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="56" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="9:10">
       <c r="J56" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="9:10">
       <c r="I59" t="s">
         <v>344</v>
       </c>
@@ -5303,7 +5266,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="60" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="9:10">
       <c r="J60" t="s">
         <v>346</v>
       </c>
@@ -5315,16 +5278,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5338,7 +5301,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5352,7 +5315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5366,7 +5329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5380,7 +5343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5400,16 +5363,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5417,7 +5380,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5425,7 +5388,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5433,7 +5396,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5447,7 +5410,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5457,22 +5420,22 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5525,7 +5488,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5535,16 +5498,16 @@
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="10.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="11" customFormat="1">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
@@ -5573,7 +5536,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -5587,29 +5550,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" customWidth="1"/>
-    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.25" customWidth="1"/>
+    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5635,6 +5598,51 @@
         <v>199</v>
       </c>
       <c r="I1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="C5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="C6" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="C7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="C9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="C10" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="C12" t="s">
         <v>194</v>
       </c>
     </row>
@@ -5644,25 +5652,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5685,7 +5693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5695,13 +5703,13 @@
       <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="9" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -5730,31 +5738,31 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="D16" s="43"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4">
       <c r="D17" s="9"/>
     </row>
   </sheetData>
@@ -5764,7 +5772,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5774,16 +5782,16 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.08984375" customWidth="1"/>
-    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.125" customWidth="1"/>
+    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="9" customFormat="1">
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
@@ -5815,8 +5823,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="15" thickBot="1"/>
+    <row r="10" spans="1:10" ht="15">
       <c r="C10" s="37" t="s">
         <v>254</v>
       </c>
@@ -5828,7 +5836,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="29.25" thickBot="1">
       <c r="C11" s="35"/>
       <c r="D11" s="38" t="s">
         <v>255</v>
@@ -5838,13 +5846,13 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10">
       <c r="H12" s="33"/>
       <c r="I12" s="34" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="15" thickBot="1">
       <c r="H13" s="35"/>
       <c r="I13" s="36" t="s">
         <v>253</v>
@@ -5856,7 +5864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5866,31 +5874,31 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.75" customWidth="1"/>
+    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="9" t="s">
         <v>249</v>
       </c>

</xml_diff>

<commit_message>
define complex net js
</commit_message>
<xml_diff>
--- a/Data/DataToCollect.xlsx
+++ b/Data/DataToCollect.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4D7E96-AF4A-4016-808E-53581180D9E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19050" windowHeight="10200" tabRatio="929" activeTab="5"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="929" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="21" r:id="rId1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="372">
   <si>
     <t>callback</t>
   </si>
@@ -1182,7 +1183,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1192,7 +1193,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1232,16 +1233,88 @@
   <si>
     <t>6. Site form to enble</t>
   </si>
+  <si>
+    <t>complex net window flow in js</t>
+  </si>
+  <si>
+    <t>1. clear all controls - in Meta Data</t>
+  </si>
+  <si>
+    <t>4. toggle to existing</t>
+  </si>
+  <si>
+    <t>2. set all toggle to new</t>
+  </si>
+  <si>
+    <t>existing ComplexNet</t>
+  </si>
+  <si>
+    <t>select ComplexNet:</t>
+  </si>
+  <si>
+    <t>save ComplexNet</t>
+  </si>
+  <si>
+    <t>1. save ComplexNet</t>
+  </si>
+  <si>
+    <t>2. toggle to existing</t>
+  </si>
+  <si>
+    <t>4. choose saved ComplexNet</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>2. all fields of the orig site should be filled except name and owner(now it is the user)</t>
+  </si>
+  <si>
+    <t>1. delete;</t>
+  </si>
+  <si>
+    <t>להוסיף ב HTML פרוייקט?</t>
+  </si>
+  <si>
+    <t>2.  change Name: text to DataList</t>
+  </si>
+  <si>
+    <t>3. set all Config and complexNet the first one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.  change Name: Data list to text </t>
+  </si>
+  <si>
+    <t>existing ComplexNet(index)</t>
+  </si>
+  <si>
+    <t>1. existing ComplexNet(selectedIndex)</t>
+  </si>
+  <si>
+    <t>3. order ComplexNet names by ABC</t>
+  </si>
+  <si>
+    <t>1. if not validate - msg</t>
+  </si>
+  <si>
+    <t>2. existing ComplexNet(1)</t>
+  </si>
+  <si>
+    <t>4.  All - Default</t>
+  </si>
+  <si>
+    <t>function ChangeComplexNetHeaders(){</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1266,7 +1339,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1486,7 +1559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1577,6 +1650,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,7 +1671,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1637,7 +1713,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1669,9 +1745,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1703,6 +1797,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1878,7 +1990,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1888,55 +2000,55 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="57" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="57" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" s="57" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="57" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" s="57" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="57"/>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" s="57" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="57" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15" thickBot="1">
+    <row r="10" spans="1:1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="58" t="s">
         <v>295</v>
       </c>
@@ -1947,7 +2059,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -1957,14 +2069,14 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1">
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -1984,7 +2096,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -1994,20 +2106,20 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" customWidth="1"/>
-    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.08984375" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:12" s="9" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>240</v>
       </c>
@@ -2039,7 +2151,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.75">
+    <row r="2" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="A2" s="13">
         <v>123</v>
       </c>
@@ -2056,7 +2168,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="19.5" thickBot="1">
+    <row r="3" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>333</v>
       </c>
@@ -2073,7 +2185,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="18.75">
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="26">
         <v>200</v>
       </c>
@@ -2090,25 +2202,25 @@
         <v>289</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75">
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="H5" s="54" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="18.75">
+    <row r="6" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="H6" s="54" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="18.75">
+    <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="H7" s="54" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="19.5" thickBot="1">
+    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="F8" s="54"/>
     </row>
-    <row r="9" spans="1:12" ht="18.75">
+    <row r="9" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="C9" s="31" t="s">
         <v>261</v>
       </c>
@@ -2117,7 +2229,7 @@
       </c>
       <c r="F9" s="54"/>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C10" s="42" t="s">
         <v>262</v>
       </c>
@@ -2125,15 +2237,15 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C11" s="55"/>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:12" ht="15" thickBot="1">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C12" s="55"/>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C13" s="44"/>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -2141,7 +2253,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="46"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C14" s="47"/>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
@@ -2154,7 +2266,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -2169,7 +2281,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
@@ -2184,7 +2296,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="3:12">
+    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
@@ -2193,7 +2305,7 @@
       <c r="H17" s="49"/>
       <c r="L17" s="16"/>
     </row>
-    <row r="18" spans="3:12">
+    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -2202,7 +2314,7 @@
       <c r="H18" s="49"/>
       <c r="L18" s="16"/>
     </row>
-    <row r="19" spans="3:12">
+    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -2210,7 +2322,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:12">
+    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -2218,7 +2330,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:12" ht="15" thickBot="1">
+    <row r="21" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="50"/>
       <c r="D21" s="51"/>
       <c r="E21" s="51"/>
@@ -2226,25 +2338,25 @@
       <c r="G21" s="51"/>
       <c r="H21" s="52"/>
     </row>
-    <row r="22" spans="3:12">
+    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C22" s="55"/>
       <c r="D22" s="20"/>
     </row>
-    <row r="23" spans="3:12">
+    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C23" s="55"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="3:12">
+    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C24" s="55"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="3:12" ht="15">
+    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
       <c r="I25" s="30" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="3:12" ht="15" thickBot="1"/>
-    <row r="27" spans="3:12">
+    <row r="26" spans="3:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C27" s="25" t="s">
         <v>240</v>
       </c>
@@ -2256,7 +2368,7 @@
       <c r="G27" s="17"/>
       <c r="H27" s="18"/>
     </row>
-    <row r="28" spans="3:12">
+    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C28" s="19"/>
       <c r="D28" s="27" t="s">
         <v>241</v>
@@ -2268,7 +2380,7 @@
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
     </row>
-    <row r="29" spans="3:12">
+    <row r="29" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28" t="s">
@@ -2282,7 +2394,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="3:12">
+    <row r="30" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2294,7 +2406,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="3:12">
+    <row r="31" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -2308,7 +2420,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="3:12">
+    <row r="32" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C32" s="19"/>
       <c r="D32" s="20"/>
       <c r="E32" s="28"/>
@@ -2322,7 +2434,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="33" spans="3:9" ht="15" thickBot="1">
+    <row r="33" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C33" s="22"/>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
@@ -2330,13 +2442,13 @@
       <c r="G33" s="23"/>
       <c r="H33" s="24"/>
     </row>
-    <row r="35" spans="3:9" ht="15">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.35">
       <c r="I35" s="30" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="36" spans="3:9" ht="15" thickBot="1"/>
-    <row r="37" spans="3:9">
+    <row r="36" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C37" s="25" t="s">
         <v>240</v>
       </c>
@@ -2348,7 +2460,7 @@
       <c r="G37" s="17"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="3:9">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C38" s="19"/>
       <c r="D38" s="27" t="s">
         <v>241</v>
@@ -2360,7 +2472,7 @@
       <c r="G38" s="20"/>
       <c r="H38" s="21"/>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C39" s="19"/>
       <c r="D39" s="20"/>
       <c r="E39" s="28" t="s">
@@ -2374,7 +2486,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="40" spans="3:9">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C40" s="19"/>
       <c r="D40" s="20"/>
       <c r="E40" s="28"/>
@@ -2386,7 +2498,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="41" spans="3:9">
+    <row r="41" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
       <c r="E41" s="28"/>
@@ -2400,7 +2512,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="3:9">
+    <row r="42" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C42" s="19"/>
       <c r="D42" s="20"/>
       <c r="E42" s="28"/>
@@ -2414,7 +2526,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="3:9">
+    <row r="43" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C43" s="19"/>
       <c r="D43" s="27" t="s">
         <v>241</v>
@@ -2426,7 +2538,7 @@
       <c r="G43" s="20"/>
       <c r="H43" s="21"/>
     </row>
-    <row r="44" spans="3:9">
+    <row r="44" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C44" s="19"/>
       <c r="D44" s="20"/>
       <c r="E44" s="28" t="s">
@@ -2440,7 +2552,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="3:9">
+    <row r="45" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C45" s="19"/>
       <c r="D45" s="20"/>
       <c r="E45" s="28"/>
@@ -2452,7 +2564,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="46" spans="3:9">
+    <row r="46" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C46" s="19"/>
       <c r="D46" s="20"/>
       <c r="E46" s="28"/>
@@ -2466,7 +2578,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="3:9" ht="15" thickBot="1">
+    <row r="47" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C47" s="22"/>
       <c r="D47" s="23"/>
       <c r="E47" s="29"/>
@@ -2480,12 +2592,12 @@
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="3:9" ht="15" thickBot="1">
+    <row r="51" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I51" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="3:9">
+    <row r="52" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C52" s="25" t="s">
         <v>240</v>
       </c>
@@ -2497,7 +2609,7 @@
       <c r="G52" s="17"/>
       <c r="H52" s="18"/>
     </row>
-    <row r="53" spans="3:9">
+    <row r="53" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C53" s="19"/>
       <c r="D53" s="27" t="s">
         <v>241</v>
@@ -2509,7 +2621,7 @@
       <c r="G53" s="20"/>
       <c r="H53" s="21"/>
     </row>
-    <row r="54" spans="3:9">
+    <row r="54" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C54" s="19"/>
       <c r="D54" s="20"/>
       <c r="E54" s="28" t="s">
@@ -2523,7 +2635,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="3:9">
+    <row r="55" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C55" s="19"/>
       <c r="D55" s="20"/>
       <c r="E55" s="28"/>
@@ -2535,7 +2647,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="3:9">
+    <row r="56" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C56" s="19"/>
       <c r="D56" s="27" t="s">
         <v>241</v>
@@ -2547,7 +2659,7 @@
       <c r="G56" s="20"/>
       <c r="H56" s="21"/>
     </row>
-    <row r="57" spans="3:9">
+    <row r="57" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C57" s="19"/>
       <c r="D57" s="20"/>
       <c r="E57" s="28" t="s">
@@ -2561,7 +2673,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="58" spans="3:9" ht="15" thickBot="1">
+    <row r="58" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C58" s="22"/>
       <c r="D58" s="23"/>
       <c r="E58" s="29"/>
@@ -2573,8 +2685,8 @@
         <v>238</v>
       </c>
     </row>
-    <row r="63" spans="3:9" ht="15" thickBot="1"/>
-    <row r="64" spans="3:9">
+    <row r="63" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="64" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C64" s="25" t="s">
         <v>240</v>
       </c>
@@ -2586,7 +2698,7 @@
       <c r="G64" s="17"/>
       <c r="H64" s="18"/>
     </row>
-    <row r="65" spans="3:8">
+    <row r="65" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C65" s="19"/>
       <c r="D65" s="20"/>
       <c r="E65" s="28" t="s">
@@ -2600,7 +2712,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="3:8">
+    <row r="66" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C66" s="19"/>
       <c r="D66" s="20"/>
       <c r="E66" s="28"/>
@@ -2612,7 +2724,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="3:8">
+    <row r="67" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C67" s="19"/>
       <c r="D67" s="20"/>
       <c r="E67" s="28"/>
@@ -2626,7 +2738,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="68" spans="3:8" ht="15" thickBot="1">
+    <row r="68" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C68" s="22"/>
       <c r="D68" s="23"/>
       <c r="E68" s="29"/>
@@ -2647,7 +2759,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2657,19 +2769,19 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1">
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>54</v>
       </c>
@@ -2698,7 +2810,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="27">
         <v>666</v>
       </c>
@@ -2710,13 +2822,13 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="I9" s="30" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1"/>
-    <row r="11" spans="1:9">
+    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" s="25" t="s">
         <v>240</v>
       </c>
@@ -2728,7 +2840,7 @@
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" s="19"/>
       <c r="D12" s="27" t="s">
         <v>241</v>
@@ -2740,7 +2852,7 @@
       <c r="G12" s="20"/>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
       <c r="E13" s="28" t="s">
@@ -2754,7 +2866,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="19"/>
       <c r="D14" s="20"/>
       <c r="E14" s="28"/>
@@ -2766,7 +2878,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
       <c r="E15" s="28"/>
@@ -2780,7 +2892,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="19"/>
       <c r="D16" s="20"/>
       <c r="E16" s="28"/>
@@ -2794,7 +2906,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="3:9" ht="15" thickBot="1">
+    <row r="17" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="22"/>
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
@@ -2802,13 +2914,13 @@
       <c r="G17" s="23"/>
       <c r="H17" s="24"/>
     </row>
-    <row r="19" spans="3:9" ht="15">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
       <c r="I19" s="30" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="20" spans="3:9" ht="15" thickBot="1"/>
-    <row r="21" spans="3:9">
+    <row r="20" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C21" s="25" t="s">
         <v>240</v>
       </c>
@@ -2820,7 +2932,7 @@
       <c r="G21" s="17"/>
       <c r="H21" s="18"/>
     </row>
-    <row r="22" spans="3:9">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C22" s="19"/>
       <c r="D22" s="27" t="s">
         <v>241</v>
@@ -2832,7 +2944,7 @@
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
     </row>
-    <row r="23" spans="3:9">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C23" s="19"/>
       <c r="D23" s="20"/>
       <c r="E23" s="28" t="s">
@@ -2846,7 +2958,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="3:9">
+    <row r="24" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C24" s="19"/>
       <c r="D24" s="20"/>
       <c r="E24" s="28"/>
@@ -2858,7 +2970,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="25" spans="3:9">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C25" s="19"/>
       <c r="D25" s="20"/>
       <c r="E25" s="28"/>
@@ -2872,7 +2984,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="26" spans="3:9">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C26" s="19"/>
       <c r="D26" s="20"/>
       <c r="E26" s="28"/>
@@ -2886,7 +2998,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="3:9">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
         <v>241</v>
@@ -2898,7 +3010,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:9">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
@@ -2912,7 +3024,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="3:9">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -2924,7 +3036,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="3:9">
+    <row r="30" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -2938,7 +3050,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="3:9" ht="15" thickBot="1">
+    <row r="31" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="29"/>
@@ -2959,7 +3071,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -2969,21 +3081,21 @@
       <selection activeCell="H3" sqref="H3:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.625" customWidth="1"/>
+    <col min="6" max="6" width="14.6328125" customWidth="1"/>
     <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3021,7 +3133,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="41">
         <v>777</v>
       </c>
@@ -3029,7 +3141,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="18.75">
+    <row r="3" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>708</v>
       </c>
@@ -3040,7 +3152,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="19.5" thickBot="1">
+    <row r="4" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>709</v>
       </c>
@@ -3051,7 +3163,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="18.75">
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>710</v>
       </c>
@@ -3062,7 +3174,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="19.5" thickBot="1">
+    <row r="6" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>710</v>
       </c>
@@ -3073,7 +3185,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="19.5" thickBot="1">
+    <row r="7" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="28">
         <v>2000</v>
       </c>
@@ -3084,7 +3196,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="19.5" thickBot="1">
+    <row r="8" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="28">
         <v>2001</v>
       </c>
@@ -3095,7 +3207,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="19.5" thickBot="1">
+    <row r="9" spans="1:12" ht="18.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="28">
         <v>2002</v>
       </c>
@@ -3106,7 +3218,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="18.75">
+    <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.4">
       <c r="A10" s="28">
         <v>2003</v>
       </c>
@@ -3120,8 +3232,8 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15" thickBot="1"/>
-    <row r="14" spans="1:12">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C14" s="44"/>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
@@ -3129,7 +3241,7 @@
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" s="47"/>
       <c r="D15" s="48"/>
       <c r="E15" s="48"/>
@@ -3139,7 +3251,7 @@
       </c>
       <c r="H15" s="49"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" s="47"/>
       <c r="D16" s="48"/>
       <c r="E16" s="48"/>
@@ -3151,7 +3263,7 @@
       </c>
       <c r="H16" s="49"/>
     </row>
-    <row r="17" spans="3:8">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C17" s="47"/>
       <c r="D17" s="48"/>
       <c r="E17" s="48"/>
@@ -3163,7 +3275,7 @@
       </c>
       <c r="H17" s="49"/>
     </row>
-    <row r="18" spans="3:8">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C18" s="47"/>
       <c r="D18" s="48"/>
       <c r="E18" s="48"/>
@@ -3171,7 +3283,7 @@
       <c r="G18" s="48"/>
       <c r="H18" s="49"/>
     </row>
-    <row r="19" spans="3:8">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
       <c r="E19" s="48"/>
@@ -3179,7 +3291,7 @@
       <c r="G19" s="48"/>
       <c r="H19" s="49"/>
     </row>
-    <row r="20" spans="3:8">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
       <c r="E20" s="48"/>
@@ -3187,7 +3299,7 @@
       <c r="G20" s="48"/>
       <c r="H20" s="49"/>
     </row>
-    <row r="21" spans="3:8">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C21" s="47"/>
       <c r="D21" s="48"/>
       <c r="E21" s="48"/>
@@ -3195,7 +3307,7 @@
       <c r="G21" s="48"/>
       <c r="H21" s="49"/>
     </row>
-    <row r="22" spans="3:8" ht="15" thickBot="1">
+    <row r="22" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C22" s="50"/>
       <c r="D22" s="51"/>
       <c r="E22" s="51"/>
@@ -3203,8 +3315,8 @@
       <c r="G22" s="51"/>
       <c r="H22" s="52"/>
     </row>
-    <row r="25" spans="3:8" ht="15" thickBot="1"/>
-    <row r="26" spans="3:8">
+    <row r="25" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C26" s="25" t="s">
         <v>240</v>
       </c>
@@ -3216,7 +3328,7 @@
       <c r="G26" s="17"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="3:8">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C27" s="19"/>
       <c r="D27" s="27" t="s">
         <v>241</v>
@@ -3228,7 +3340,7 @@
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
     </row>
-    <row r="28" spans="3:8">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C28" s="19"/>
       <c r="D28" s="20"/>
       <c r="E28" s="28" t="s">
@@ -3242,7 +3354,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="3:8">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C29" s="19"/>
       <c r="D29" s="20"/>
       <c r="E29" s="28"/>
@@ -3254,7 +3366,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="3:8">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C30" s="19"/>
       <c r="D30" s="20"/>
       <c r="E30" s="28"/>
@@ -3268,7 +3380,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="3:8">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C31" s="19"/>
       <c r="D31" s="20"/>
       <c r="E31" s="28"/>
@@ -3282,7 +3394,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="3:8" ht="15" thickBot="1">
+    <row r="32" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C32" s="22"/>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
@@ -3290,8 +3402,8 @@
       <c r="G32" s="23"/>
       <c r="H32" s="24"/>
     </row>
-    <row r="35" spans="3:8" ht="15" thickBot="1"/>
-    <row r="36" spans="3:8">
+    <row r="35" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C36" s="25" t="s">
         <v>240</v>
       </c>
@@ -3303,7 +3415,7 @@
       <c r="G36" s="17"/>
       <c r="H36" s="18"/>
     </row>
-    <row r="37" spans="3:8">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C37" s="19"/>
       <c r="D37" s="28" t="s">
         <v>242</v>
@@ -3317,7 +3429,7 @@
       </c>
       <c r="H37" s="21"/>
     </row>
-    <row r="38" spans="3:8">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C38" s="19"/>
       <c r="D38" s="28"/>
       <c r="E38" s="28">
@@ -3328,7 +3440,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="39" spans="3:8">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C39" s="19"/>
       <c r="D39" s="28"/>
       <c r="E39" s="28">
@@ -3341,7 +3453,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="40" spans="3:8">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C40" s="19"/>
       <c r="D40" s="28"/>
       <c r="E40" s="28">
@@ -3354,11 +3466,11 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="3:8">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C41" s="19"/>
       <c r="D41" s="20"/>
     </row>
-    <row r="42" spans="3:8" ht="15" thickBot="1">
+    <row r="42" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C42" s="22"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -3373,28 +3485,28 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -3426,7 +3538,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3458,7 +3570,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3490,7 +3602,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -3522,7 +3634,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -3554,7 +3666,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -3586,7 +3698,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3618,7 +3730,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3650,7 +3762,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3682,34 +3794,34 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:10" ht="15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="3:3" ht="15">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C17" s="3"/>
     </row>
-    <row r="18" spans="3:3" ht="15">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="3:3" ht="15">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C19" s="3"/>
     </row>
-    <row r="20" spans="3:3" ht="15">
+    <row r="20" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="3:3" ht="15">
+    <row r="21" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C21" s="3"/>
     </row>
-    <row r="22" spans="3:3" ht="15">
+    <row r="22" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="3:3" ht="15">
+    <row r="23" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C23" s="3"/>
     </row>
-    <row r="24" spans="3:3" ht="15">
+    <row r="24" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C24" s="3"/>
     </row>
   </sheetData>
@@ -3719,23 +3831,23 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.75" customWidth="1"/>
-    <col min="5" max="5" width="15.875" customWidth="1"/>
-    <col min="6" max="6" width="22.25" customWidth="1"/>
+    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15.90625" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>54</v>
       </c>
@@ -3755,7 +3867,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="4">
         <v>1</v>
@@ -3773,7 +3885,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="4">
         <v>1</v>
@@ -3791,7 +3903,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4">
         <v>2</v>
@@ -3809,7 +3921,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4">
         <v>3</v>
@@ -3827,7 +3939,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4">
         <v>4</v>
@@ -3845,7 +3957,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="B7" s="4">
         <v>5</v>
@@ -3863,7 +3975,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
         <v>2</v>
       </c>
@@ -3880,7 +3992,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>3</v>
       </c>
@@ -3897,7 +4009,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>3</v>
       </c>
@@ -3920,32 +4032,32 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.375" customWidth="1"/>
-    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.36328125" customWidth="1"/>
+    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4004,7 +4116,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4060,7 +4172,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4116,7 +4228,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4170,7 +4282,7 @@
       </c>
       <c r="S4" s="6"/>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4223,7 +4335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4276,7 +4388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4329,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4383,7 +4495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4444,19 +4556,19 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4467,7 +4579,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4475,7 +4587,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4483,7 +4595,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4491,7 +4603,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4505,16 +4617,16 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4525,7 +4637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4533,7 +4645,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4541,7 +4653,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4549,7 +4661,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4563,16 +4675,16 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4592,7 +4704,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4612,7 +4724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4632,7 +4744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4652,7 +4764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4672,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4692,7 +4804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4712,7 +4824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4732,7 +4844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4752,7 +4864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4772,7 +4884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4792,7 +4904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4812,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -4832,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4852,7 +4964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4872,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4892,7 +5004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4912,7 +5024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4938,26 +5050,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:J60"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7:J60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.75" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -4977,7 +5089,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4990,7 +5102,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5003,7 +5115,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5016,7 +5128,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5029,22 +5141,22 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G7" s="13" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H8" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="I9" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H12" t="s">
         <v>307</v>
       </c>
@@ -5052,65 +5164,65 @@
         <v>305</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J13" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J14" s="8" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J15" s="8" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J16" s="8" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="9:10">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J17" s="11"/>
     </row>
-    <row r="18" spans="9:10">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I18" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="19" spans="9:10">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J19" s="8" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="9:10">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J20" s="8" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="21" spans="9:10">
+    <row r="21" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J21" s="8" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="22" spans="9:10">
+    <row r="22" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J22" s="8" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="23" spans="9:10">
+    <row r="23" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I23" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="9:10">
+    <row r="24" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J24" s="8" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="26" spans="9:10">
+    <row r="26" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I26" t="s">
         <v>328</v>
       </c>
@@ -5118,32 +5230,32 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="9:10">
+    <row r="27" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J27" s="8" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="28" spans="9:10">
+    <row r="28" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J28" s="11" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="9:10">
+    <row r="29" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J29" s="8" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="30" spans="9:10">
+    <row r="30" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J30" s="8" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="9:10">
+    <row r="31" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J31" s="8" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="33" spans="3:10">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C33" s="59"/>
       <c r="D33" s="59"/>
       <c r="E33" s="59"/>
@@ -5157,72 +5269,72 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="3:10">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J34" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="35" spans="3:10">
+    <row r="35" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J35" s="8" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="36" spans="3:10">
+    <row r="36" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J36" s="8" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="3:10">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
       <c r="I38" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="39" spans="3:10">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J39" s="8" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="40" spans="3:10">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J40" s="8" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="41" spans="3:10">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J41" s="8" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="42" spans="3:10">
+    <row r="42" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J42" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="43" spans="3:10">
+    <row r="43" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J43" s="11" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="44" spans="3:10" ht="15">
+    <row r="44" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J44" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="46" spans="3:10">
+    <row r="46" spans="3:10" x14ac:dyDescent="0.35">
       <c r="I46" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="47" spans="3:10">
+    <row r="47" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J47" s="8" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="48" spans="3:10">
+    <row r="48" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J48" s="8" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="9:10">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I50" t="s">
         <v>119</v>
       </c>
@@ -5230,22 +5342,22 @@
         <v>338</v>
       </c>
     </row>
-    <row r="51" spans="9:10">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J51" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="9:10">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J52" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="53" spans="9:10">
+    <row r="53" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J53" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="55" spans="9:10">
+    <row r="55" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I55" t="s">
         <v>342</v>
       </c>
@@ -5253,12 +5365,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="56" spans="9:10">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J56" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="59" spans="9:10">
+    <row r="59" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I59" t="s">
         <v>344</v>
       </c>
@@ -5266,7 +5378,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="60" spans="9:10">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.35">
       <c r="J60" t="s">
         <v>346</v>
       </c>
@@ -5278,16 +5390,16 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5301,7 +5413,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5315,7 +5427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5329,7 +5441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5343,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5363,16 +5475,16 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5380,7 +5492,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5388,7 +5500,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5396,7 +5508,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5410,7 +5522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5420,22 +5532,22 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.36328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5488,26 +5600,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
-    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="72.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="11" customFormat="1">
+    <row r="1" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>54</v>
       </c>
@@ -5536,7 +5650,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -5544,13 +5658,210 @@
       <c r="F2" s="9"/>
       <c r="G2" s="9"/>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G3" s="60" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D4" s="13" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G10" s="11" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G11" s="11" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G12" s="11" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G13" s="11" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G17" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="18" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G18" s="8" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="19" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G19" s="8" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G20" s="8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="21" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F22" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G23" s="11" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G24" s="11"/>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>354</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G27" s="11" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="11" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G29" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>342</v>
+      </c>
+      <c r="G32" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="G33" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="F36" t="s">
+        <v>344</v>
+      </c>
+      <c r="G36" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.35">
+      <c r="G37" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>358</v>
+      </c>
+      <c r="G40" t="s">
+        <v>360</v>
+      </c>
+      <c r="H40"/>
+      <c r="I40"/>
+    </row>
+    <row r="41" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F41"/>
+      <c r="G41" t="s">
+        <v>369</v>
+      </c>
+      <c r="H41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="6:9" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="51" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="52" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="58" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="61" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="62" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="63" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="64" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="65" s="11" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5560,19 +5871,19 @@
       <selection activeCell="C4" sqref="C4:C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.25" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" customWidth="1"/>
+    <col min="8" max="8" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5601,47 +5912,47 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>194</v>
       </c>
@@ -5652,25 +5963,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -5693,7 +6004,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5703,13 +6014,13 @@
       <selection activeCell="B1" sqref="B1:I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="9" customFormat="1">
+    <row r="1" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
         <v>54</v>
       </c>
@@ -5738,31 +6049,31 @@
         <v>186</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" s="43"/>
     </row>
-    <row r="17" spans="4:4">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D17" s="9"/>
     </row>
   </sheetData>
@@ -5772,7 +6083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5782,16 +6093,16 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.125" customWidth="1"/>
-    <col min="10" max="10" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" customWidth="1"/>
+    <col min="10" max="10" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="9" customFormat="1">
+    <row r="1" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>54</v>
       </c>
@@ -5823,8 +6134,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1"/>
-    <row r="10" spans="1:10" ht="15">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C10" s="37" t="s">
         <v>254</v>
       </c>
@@ -5836,7 +6147,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="29.25" thickBot="1">
+    <row r="11" spans="1:10" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C11" s="35"/>
       <c r="D11" s="38" t="s">
         <v>255</v>
@@ -5846,13 +6157,13 @@
         <v>251</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="H12" s="33"/>
       <c r="I12" s="34" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="H13" s="35"/>
       <c r="I13" s="36" t="s">
         <v>253</v>
@@ -5864,7 +6175,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="-0.249977111117893"/>
   </sheetPr>
@@ -5874,31 +6185,31 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="2" max="2" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.08984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.08984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1">
+    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>249</v>
       </c>

</xml_diff>